<commit_message>
Menu de navegacion con Hipervinculos
</commit_message>
<xml_diff>
--- a/empresa.xlsx
+++ b/empresa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xls-mjv13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69409F2D-016C-448C-9564-958F08D4D594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B25775-E7D2-4B3F-9D62-8B6FCB515047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="487" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="año_actual">empleados!$O$2</definedName>
-    <definedName name="char">Datos!$G$2</definedName>
+    <definedName name="char">Datos!$H$2</definedName>
     <definedName name="fecha_actual">empleados!$M$2</definedName>
     <definedName name="iva_ventas">ventas!$K$1</definedName>
   </definedNames>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="153">
   <si>
     <t>Apellido</t>
   </si>
@@ -496,6 +496,12 @@
   </si>
   <si>
     <t>atrás</t>
+  </si>
+  <si>
+    <t>Datos</t>
+  </si>
+  <si>
+    <t>Intro</t>
   </si>
 </sst>
 </file>
@@ -674,7 +680,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -735,12 +741,18 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1090,6 +1102,1414 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>42447</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>39413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>25014</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>54067</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8077A5D7-DE18-4D6B-9A8F-4F3304061BBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a14:imgLayer r:embed="rId2">
+                  <a14:imgEffect>
+                    <a14:backgroundRemoval t="10000" b="90000" l="10000" r="90000">
+                      <a14:foregroundMark x1="31111" y1="26667" x2="26222" y2="67556"/>
+                      <a14:backgroundMark x1="15556" y1="7556" x2="83111" y2="14222"/>
+                    </a14:backgroundRemoval>
+                  </a14:imgEffect>
+                  <a14:imgEffect>
+                    <a14:colorTemperature colorTemp="4700"/>
+                  </a14:imgEffect>
+                  <a14:imgEffect>
+                    <a14:saturation sat="66000"/>
+                  </a14:imgEffect>
+                </a14:imgLayer>
+              </a14:imgProps>
+            </a:ext>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="13194" t="15135" r="10682" b="15676"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4864068" y="801413"/>
+          <a:ext cx="1125567" cy="967154"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>26362</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>31398</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>748159</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>749436</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99502639-26BA-405E-82FB-50A9A83DB67A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent1">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{837473B0-CC2E-450A-ABE3-18F120FF3D39}">
+              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" r:id="rId5"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="23149" t="-216" r="24076" b="216"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3323983" y="983898"/>
+          <a:ext cx="721797" cy="718038"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542191</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>109318</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1055077" cy="514949"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="CuadroTexto 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9260CB85-D2E7-4BF1-BCC3-0A4EED3EA405}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3077306" y="5062318"/>
+          <a:ext cx="1055077" cy="514949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-AR" sz="900">
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5" tooltip="http://informationtransfereconomics.blogspot.com/2017/02/information-equilibrium-code.html"/>
+            </a:rPr>
+            <a:t>Esta foto</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="900"/>
+            <a:t> de Autor desconocido está bajo licencia </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-AR" sz="900">
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6" tooltip="https://creativecommons.org/licenses/by/3.0/"/>
+            </a:rPr>
+            <a:t>CC BY</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-AR" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>59872</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>59121</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>707872</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>709448</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="14" name="Grupo 13">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBA665E1-826F-46DD-8AE3-5BCC3E340EBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3357493" y="1011621"/>
+          <a:ext cx="648000" cy="650327"/>
+          <a:chOff x="2596243" y="1011621"/>
+          <a:chExt cx="648000" cy="650327"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Triángulo isósceles 9">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{237492C4-6460-47E5-9E7B-83C93FF949EE}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2815999" y="1182414"/>
+            <a:ext cx="428244" cy="472965"/>
+          </a:xfrm>
+          <a:prstGeom prst="triangle">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-AR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="13" name="Grupo 12">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCC26A3D-026F-45C8-AE4B-2238DD665979}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2596243" y="1011621"/>
+            <a:ext cx="489857" cy="650327"/>
+            <a:chOff x="2596243" y="1011621"/>
+            <a:chExt cx="489857" cy="650327"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="Paralelogramo 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43AF4F17-B3AE-44AD-B7DC-5D78267E3490}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2596243" y="1011621"/>
+              <a:ext cx="445148" cy="650327"/>
+            </a:xfrm>
+            <a:prstGeom prst="parallelogram">
+              <a:avLst>
+                <a:gd name="adj" fmla="val 72111"/>
+              </a:avLst>
+            </a:prstGeom>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="es-AR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="Triángulo isósceles 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93738D76-3A9B-4AB7-8BBF-5C638E0E6F92}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2775857" y="1240970"/>
+              <a:ext cx="310243" cy="315875"/>
+            </a:xfrm>
+            <a:prstGeom prst="triangle">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="es-AR" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203818</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19707</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>922327</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>739707</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Gráfico 16" descr="Hogar con relleno sólido">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76D2EF20-7EC0-4FA2-ACF5-5A76F74FBE9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5025439" y="19707"/>
+          <a:ext cx="718509" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>623252</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>727212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>41252</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>145212</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Gráfico 18" descr="Atrás con relleno sólido">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF686EA2-8158-4431-8FB1-20E9B3F6A720}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId11"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5825873" y="727212"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>43239</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>43239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1239</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1239</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Gráfico 20" descr="Lápiz con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A014007C-0406-4B24-9F57-575E92F2ECF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId14"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1815717" y="995739"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19304</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>27587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>739304</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>747587</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Gráfico 22" descr="Correo electrónico con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD08A190-9E70-4AFF-A8B3-45B09D1B7BA2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId17"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1029782" y="980087"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>20217</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>53348</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>740217</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>11348</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Gráfico 24" descr="Documento con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA1FFC59-70E4-48E4-943C-13B3CDA4CBEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId20"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="268695" y="1005848"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7707</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>21416</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>727707</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>741416</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Gráfico 26" descr="Tendencia al alza con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1AD432C-FCC0-417E-A9D4-37F00040CBEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId23"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3305328" y="21416"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28613</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>50319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>748613</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>8319</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Gráfico 28" descr="Dinero con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA6084AA-F53F-468A-9B32-1E695426584A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId26"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2564234" y="50319"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>26384</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>124347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>746384</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>82347</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Gráfico 30" descr="Camión con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAA7C475-B37A-4CCE-B2D4-940C1D262ACF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId29"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1800005" y="124347"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>17300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>737300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>720000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Gráfico 32" descr="Lista con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24F3F5FD-BAC2-44B2-BB0B-6FFDFEBE3E1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId32"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028921" y="0"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>29638</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>749638</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>748211</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Gráfico 34" descr="Identificación de empleado con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D05D4C4E-113F-4FC2-A953-6E2C58AEB2CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId35"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="279259" y="28211"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>65690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>726569</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95949</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Gráfico 36" descr="Maestro con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7EC6615-3B9D-4625-963F-E79BA1A97CBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId38"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1780190" y="1018190"/>
+          <a:ext cx="720000" cy="792259"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>18622</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>32845</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>738622</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>752845</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Gráfico 38" descr="Base de datos con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF5AC3CF-96E8-4D64-933D-5F14965FCE03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId41"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1792243" y="32845"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>41672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>221672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51566A93-CD6C-405F-8330-9C001880D73F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="41672" y="5953"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>41672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>221672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33A9F8D-2ABF-4A55-AA7E-0BDEAE59C322}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="41672" y="5953"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>374570</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>208575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>554570</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5E6C6AF-DD3F-4AF2-B521-08A15E93FBA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="28575" y="374570"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>41672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>221672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F54E7848-5AE7-4C4C-9124-8375E246E700}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="41672" y="5953"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>41672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>221672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E43168FF-7D10-4FB7-9DF8-C368ACC2001F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="41672" y="5953"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>41672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>221672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>185953</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B1C1AA-53DA-485F-A9C4-7BCBE10ACA38}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="41672" y="5953"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FAF7F421-A303-4292-9998-E17312DF5C4D}" name="tabla_empleados" displayName="tabla_empleados" comment="Informacion del Personal de la Empresa" ref="B1:K9" totalsRowShown="0">
   <autoFilter ref="B1:K9" xr:uid="{FAF7F421-A303-4292-9998-E17312DF5C4D}"/>
@@ -1118,8 +2538,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CADF3F30-502A-4F21-BCA4-ECFD83EEB22A}" name="tabla_datos" displayName="tabla_datos" comment="Tabla con extraccion de Nombre y apellido de Empleados" ref="A1:E9" totalsRowShown="0">
-  <autoFilter ref="A1:E9" xr:uid="{CADF3F30-502A-4F21-BCA4-ECFD83EEB22A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CADF3F30-502A-4F21-BCA4-ECFD83EEB22A}" name="tabla_datos" displayName="tabla_datos" comment="Tabla con extraccion de Nombre y apellido de Empleados" ref="B1:F9" totalsRowShown="0">
+  <autoFilter ref="B1:F9" xr:uid="{CADF3F30-502A-4F21-BCA4-ECFD83EEB22A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{29B4FC90-C2F0-4B58-BFFA-F95ED0272441}" name="Empleado">
       <calculatedColumnFormula>TRIM(presentismo!B2)</calculatedColumnFormula>
@@ -1472,62 +2892,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B73CBFC-728A-4FAD-AF56-CCF163A7BEB8}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" s="46"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="E2" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="F2" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="G2" s="49" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="46"/>
+    </row>
+    <row r="3" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="46"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="49" t="s">
         <v>146</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="F4" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="G4" s="49" t="s">
         <v>149</v>
       </c>
+      <c r="H4" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1537,16 +2974,19 @@
   <hyperlinks>
     <hyperlink ref="B2" location="empleados!A1" display="Empleados" xr:uid="{8FD0F67B-0881-439C-9B4F-54C2A8484AA9}"/>
     <hyperlink ref="C2" location="presentismo!A1" display="Asistencia" xr:uid="{471CC1BE-FEBC-4201-B514-4678289F0B6C}"/>
-    <hyperlink ref="D2" location="productos!A1" display="Productos" xr:uid="{233EA16B-6356-446D-B3AB-846315C8DBA2}"/>
-    <hyperlink ref="E2" location="ventas!A1" display="Ventas" xr:uid="{2A2E4FDB-9636-456E-8F57-637A5722BD88}"/>
-    <hyperlink ref="F2" location="estadisticas!A1" display="Estadisticas" xr:uid="{9AA00A8F-A601-4768-8A9A-4160D2C4C3C7}"/>
+    <hyperlink ref="E2" location="productos!A1" display="Productos" xr:uid="{233EA16B-6356-446D-B3AB-846315C8DBA2}"/>
+    <hyperlink ref="F2" location="ventas!A1" display="Ventas" xr:uid="{2A2E4FDB-9636-456E-8F57-637A5722BD88}"/>
+    <hyperlink ref="G2" location="estadisticas!A1" display="Estadisticas" xr:uid="{9AA00A8F-A601-4768-8A9A-4160D2C4C3C7}"/>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{573A89D0-82F4-4530-BE07-49F82FCB2F4D}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{2C0E0674-11CA-43DD-8164-972B84133705}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{C4A47B32-ED93-43FC-932A-E249AECE7D9F}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{93934089-63E0-4589-9A50-51B80B978C11}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{12B07B36-8EA2-46DA-BB99-D9FA342E582F}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{C4A47B32-ED93-43FC-932A-E249AECE7D9F}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{93934089-63E0-4589-9A50-51B80B978C11}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{12B07B36-8EA2-46DA-BB99-D9FA342E582F}"/>
+    <hyperlink ref="D2" location="Datos!A1" display="Datos" xr:uid="{E18D4BFF-FE9D-4737-9DAE-DD971379E1F0}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{F43857B0-7367-48EA-A3C3-68B996FAA8A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1554,15 +2994,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
@@ -1584,7 +3024,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>150</v>
       </c>
       <c r="B1" t="s">
@@ -1683,7 +3123,7 @@
       </c>
       <c r="N2" s="43">
         <f ca="1">NOW()</f>
-        <v>44910.699760416668</v>
+        <v>44910.732506134256</v>
       </c>
       <c r="O2" s="6">
         <f ca="1">YEAR(fecha_actual)</f>
@@ -1699,15 +3139,15 @@
       </c>
       <c r="R2" s="6">
         <f ca="1">HOUR(N2)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S2" s="6">
         <f ca="1">MINUTE(N2)</f>
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="T2" s="19">
         <f ca="1">SECOND(N2)</f>
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2003,231 +3443,238 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C368CA-EC1F-4C28-88F2-7559A5997862}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="50"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>107</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="str">
         <f>TRIM(presentismo!B2)</f>
         <v>Racedo, Cristian</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2" t="str">
         <f>RIGHT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[largo]]-(tabla_datos[[#This Row],[posicion]] + 1))</f>
         <v>Cristian</v>
       </c>
-      <c r="C2" t="str">
+      <c r="D2" t="str">
         <f>LEFT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[posicion]]-1)</f>
         <v>Racedo</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <f>FIND(char,tabla_datos[[#This Row],[Empleado]])</f>
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <f>LEN(tabla_datos[[#This Row],[Empleado]])</f>
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="str">
         <f>TRIM(presentismo!B3)</f>
         <v>Racedo, Abel</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C3" t="str">
         <f>RIGHT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[largo]]-(tabla_datos[[#This Row],[posicion]] + 1))</f>
         <v>Abel</v>
       </c>
-      <c r="C3" t="str">
+      <c r="D3" t="str">
         <f>LEFT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[posicion]]-1)</f>
         <v>Racedo</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f>FIND(char,tabla_datos[[#This Row],[Empleado]])</f>
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <f>LEN(tabla_datos[[#This Row],[Empleado]])</f>
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="str">
         <f>TRIM(presentismo!B4)</f>
         <v>Maldonado, Alejandra</v>
       </c>
-      <c r="B4" t="str">
+      <c r="C4" t="str">
         <f>RIGHT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[largo]]-(tabla_datos[[#This Row],[posicion]] + 1))</f>
         <v>Alejandra</v>
       </c>
-      <c r="C4" t="str">
+      <c r="D4" t="str">
         <f>LEFT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[posicion]]-1)</f>
         <v>Maldonado</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f>FIND(char,tabla_datos[[#This Row],[Empleado]])</f>
         <v>10</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <f>LEN(tabla_datos[[#This Row],[Empleado]])</f>
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
         <f>TRIM(presentismo!B5)</f>
         <v>Juarez, Alberto</v>
       </c>
-      <c r="B5" t="str">
+      <c r="C5" t="str">
         <f>RIGHT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[largo]]-(tabla_datos[[#This Row],[posicion]] + 1))</f>
         <v>Alberto</v>
       </c>
-      <c r="C5" t="str">
+      <c r="D5" t="str">
         <f>LEFT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[posicion]]-1)</f>
         <v>Juarez</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <f>FIND(char,tabla_datos[[#This Row],[Empleado]])</f>
         <v>7</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <f>LEN(tabla_datos[[#This Row],[Empleado]])</f>
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
         <f>TRIM(presentismo!B6)</f>
         <v>Martinez, Mariana</v>
       </c>
-      <c r="B6" t="str">
+      <c r="C6" t="str">
         <f>RIGHT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[largo]]-(tabla_datos[[#This Row],[posicion]] + 1))</f>
         <v>Mariana</v>
       </c>
-      <c r="C6" t="str">
+      <c r="D6" t="str">
         <f>LEFT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[posicion]]-1)</f>
         <v>Martinez</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <f>FIND(char,tabla_datos[[#This Row],[Empleado]])</f>
         <v>9</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <f>LEN(tabla_datos[[#This Row],[Empleado]])</f>
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
         <f>TRIM(presentismo!B7)</f>
         <v>Gomez, Graciela</v>
       </c>
-      <c r="B7" t="str">
+      <c r="C7" t="str">
         <f>RIGHT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[largo]]-(tabla_datos[[#This Row],[posicion]] + 1))</f>
         <v>Graciela</v>
       </c>
-      <c r="C7" t="str">
+      <c r="D7" t="str">
         <f>LEFT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[posicion]]-1)</f>
         <v>Gomez</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f>FIND(char,tabla_datos[[#This Row],[Empleado]])</f>
         <v>6</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f>LEN(tabla_datos[[#This Row],[Empleado]])</f>
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="str">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
         <f>TRIM(presentismo!B8)</f>
         <v>Garcia, Demetrio</v>
       </c>
-      <c r="B8" t="str">
+      <c r="C8" t="str">
         <f>RIGHT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[largo]]-(tabla_datos[[#This Row],[posicion]] + 1))</f>
         <v>Demetrio</v>
       </c>
-      <c r="C8" t="str">
+      <c r="D8" t="str">
         <f>LEFT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[posicion]]-1)</f>
         <v>Garcia</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f>FIND(char,tabla_datos[[#This Row],[Empleado]])</f>
         <v>7</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f>LEN(tabla_datos[[#This Row],[Empleado]])</f>
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="str">
         <f>TRIM(presentismo!B9)</f>
         <v>Cabello, Camila</v>
       </c>
-      <c r="B9" t="str">
+      <c r="C9" t="str">
         <f>RIGHT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[largo]]-(tabla_datos[[#This Row],[posicion]] + 1))</f>
         <v>Camila</v>
       </c>
-      <c r="C9" t="str">
+      <c r="D9" t="str">
         <f>LEFT(tabla_datos[[#This Row],[Empleado]],tabla_datos[[#This Row],[posicion]]-1)</f>
         <v>Cabello</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f>FIND(char,tabla_datos[[#This Row],[Empleado]])</f>
         <v>8</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f>LEN(tabla_datos[[#This Row],[Empleado]])</f>
         <v>15</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="menu!A1" display="atrás" xr:uid="{52F5A465-28D2-48CE-B5A6-F404D2F6AE0E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2236,16 +3683,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AL31"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="45" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.7109375" style="18" bestFit="1" customWidth="1"/>
@@ -3155,10 +4602,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="menu!A1" display="atrás" xr:uid="{8A76C932-1168-442B-BE54-5E2A24977812}"/>
+    <hyperlink ref="A1" location="menu!A1" display="Volver" xr:uid="{6C2EC084-3FEA-47B0-BB6A-501CCE8EF332}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3173,7 +4621,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -3182,7 +4630,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>150</v>
       </c>
       <c r="B1" t="s">
@@ -3339,11 +4787,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="menu!A1" display="Volver" xr:uid="{40C2321A-D476-4392-AE61-3EA790DD9B38}"/>
+    <hyperlink ref="A1" location="menu!A1" display="Volver" xr:uid="{ECEF68EC-BB86-47EE-B0F0-A293ECFB4325}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3359,7 +4808,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
@@ -3373,7 +4822,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>150</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -3830,11 +5279,12 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="menu!A1" display="Volver" xr:uid="{A2747F96-F73A-47F1-8C49-82AA64078E0A}"/>
+    <hyperlink ref="A1" location="menu!A1" display="Volver" xr:uid="{261F7D50-C145-4C27-AC5E-50FB264B982C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3843,25 +5293,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956760E-99C3-4188-ABA4-1CAAD0DD9EC6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>150</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="menu!A1" display="Volver" xr:uid="{A91A2388-E58F-4E26-9A2B-ACFAE4BB8D1C}"/>
+    <hyperlink ref="A1" location="menu!A1" display="Volver" xr:uid="{D14498A6-7B24-4ABE-88AB-4CFAB7CF46A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Funciones de Fechas y referencias
</commit_message>
<xml_diff>
--- a/empresa.xlsx
+++ b/empresa.xlsx
@@ -8,18 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xls-v10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9466853C-68AE-4BA2-BF48-C6CA0A4FFCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9B1A19-643B-4089-B1C5-499A7D73E950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{FBF13C54-EAF5-48F7-B675-6702B08EF7EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBF13C54-EAF5-48F7-B675-6702B08EF7EF}"/>
   </bookViews>
   <sheets>
     <sheet name="empleados" sheetId="1" r:id="rId1"/>
-    <sheet name="presentismo" sheetId="4" r:id="rId2"/>
-    <sheet name="productos" sheetId="2" r:id="rId3"/>
-    <sheet name="ventas" sheetId="3" r:id="rId4"/>
+    <sheet name="datos" sheetId="5" r:id="rId2"/>
+    <sheet name="presentismo" sheetId="4" r:id="rId3"/>
+    <sheet name="productos" sheetId="2" r:id="rId4"/>
+    <sheet name="ventas" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="ahora">datos!$P$2</definedName>
+    <definedName name="año">datos!$Q$2</definedName>
     <definedName name="cant">ventas!$D:$D</definedName>
+    <definedName name="hoy">datos!$O$2</definedName>
     <definedName name="iva">ventas!$J$2</definedName>
     <definedName name="precio">ventas!$E:$E</definedName>
     <definedName name="precio_iva">ventas!$G:$G</definedName>
@@ -43,8 +47,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="98">
   <si>
     <t>codigo</t>
   </si>
@@ -58,9 +84,6 @@
     <t>legajo</t>
   </si>
   <si>
-    <t>fecha nac</t>
-  </si>
-  <si>
     <t>edad</t>
   </si>
   <si>
@@ -70,21 +93,12 @@
     <t>cuil</t>
   </si>
   <si>
-    <t>racedo</t>
-  </si>
-  <si>
-    <t>cristian</t>
-  </si>
-  <si>
     <t>cdr18491</t>
   </si>
   <si>
     <t>7g</t>
   </si>
   <si>
-    <t>abel</t>
-  </si>
-  <si>
     <t>aar121093</t>
   </si>
   <si>
@@ -118,12 +132,6 @@
     <t>cant</t>
   </si>
   <si>
-    <t>Aguilera</t>
-  </si>
-  <si>
-    <t>Cristina</t>
-  </si>
-  <si>
     <t>ace85939</t>
   </si>
   <si>
@@ -257,18 +265,119 @@
   </si>
   <si>
     <t>Suma</t>
+  </si>
+  <si>
+    <t>27-45241471-1</t>
+  </si>
+  <si>
+    <t>23-33016244-9</t>
+  </si>
+  <si>
+    <t>Osses</t>
+  </si>
+  <si>
+    <t>osa18329</t>
+  </si>
+  <si>
+    <t>mla9120</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>10s</t>
+  </si>
+  <si>
+    <t>HOY</t>
+  </si>
+  <si>
+    <t>AHORA</t>
+  </si>
+  <si>
+    <t>AÑO</t>
+  </si>
+  <si>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>años</t>
+  </si>
+  <si>
+    <t>nacimiento</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>docmento</t>
+  </si>
+  <si>
+    <t>empleado</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>largo</t>
+  </si>
+  <si>
+    <t>cristian Damian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">racedo    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    racedo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Aguilera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cristina     </t>
+  </si>
+  <si>
+    <t>Abel      Alejandro</t>
+  </si>
+  <si>
+    <t>Shakira      Alejandra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lionel      Andres </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Messi    </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$$-2C0A]\ * #,##0.00_-;\-[$$-2C0A]\ * #,##0.00_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +388,22 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -297,16 +422,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -314,33 +463,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -350,12 +531,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
+    <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="52">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -459,12 +654,319 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="d/m/yy;@"/>
-      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="d/m/yy;@"/>
+      <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
+      <alignment horizontal="center" vertical="center" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
       <alignment horizontal="center" vertical="center" textRotation="75" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
@@ -488,25 +990,97 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}" name="empleados" displayName="empleados" ref="A1:H4" totalsRowShown="0">
-  <autoFilter ref="A1:H4" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}" name="empleados" displayName="empleados" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9B2FABCB-122E-4021-BCB9-1ABCF38F08D1}" name="codigo"/>
     <tableColumn id="2" xr3:uid="{48BCCCB0-2E0A-4212-A44B-A72FF9EFADA4}" name="apellido"/>
     <tableColumn id="3" xr3:uid="{8E2D81A4-6B1C-4EE6-B057-EC49A27E5F85}" name="nombre"/>
     <tableColumn id="4" xr3:uid="{FAD0BCDF-63FA-416C-A9FA-7BBA19E4DC2A}" name="legajo"/>
-    <tableColumn id="5" xr3:uid="{FDC1831B-A431-4700-AA4A-2FBE0A96C27E}" name="fecha nac" dataDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{688A04DA-9A69-41C2-B220-48FBDD3AA266}" name="edad"/>
     <tableColumn id="7" xr3:uid="{B0450268-4DC5-4E02-B6A4-0DBA5EAA50A9}" name="sector"/>
-    <tableColumn id="8" xr3:uid="{926D684E-B855-4F94-973A-B6231FEF889B}" name="cuil"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}" name="presentismo" displayName="presentismo" ref="A1:AG4" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A1:AG4" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{21CB7767-E429-4D32-8B4C-B110EB0BC09A}" name="tiempo" displayName="tiempo" ref="O1:V2" totalsRowShown="0">
+  <autoFilter ref="O1:V2" xr:uid="{21CB7767-E429-4D32-8B4C-B110EB0BC09A}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{D0C157DB-5866-4540-85DA-CA9246E3491C}" name="HOY" dataDxfId="51">
+      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{F19B6CA2-44B0-4AA2-94E5-4821559CF825}" name="AHORA" dataDxfId="50">
+      <calculatedColumnFormula>NOW()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E5C1B772-C41D-4F28-BDF3-44DE9CE5F354}" name="AÑO">
+      <calculatedColumnFormula>YEAR(hoy)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{D7A2B56F-CDB5-46FE-9F3A-B53F8B320C2C}" name="MES">
+      <calculatedColumnFormula>MONTH(hoy)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{BD792C6E-D733-4276-A139-0625F542E532}" name="DIA">
+      <calculatedColumnFormula>DAY(hoy)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C6D520E3-FDB5-4362-891A-E0FCD1A160A0}" name="HH">
+      <calculatedColumnFormula>HOUR(ahora)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{7D86770F-F4B1-43B7-B02B-F17DA43F123F}" name="mm">
+      <calculatedColumnFormula>MINUTE(ahora)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{C4C57FCE-EDF1-4327-A274-435F95FB651D}" name="ss">
+      <calculatedColumnFormula>SECOND(ahora)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A8CA9039-9259-406D-B167-9DC94801EDAB}" name="datos" displayName="datos" ref="A1:M6" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="A1:M6" xr:uid="{A8CA9039-9259-406D-B167-9DC94801EDAB}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{1E40E760-3B7A-46CB-ADE6-9C36221D8FBE}" name="empleado" dataDxfId="47">
+      <calculatedColumnFormula>TRIM(presentismo[[#This Row],[Empleado]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{A673056C-D666-4A82-8F15-DA591ECD51CD}" name="apellido" dataDxfId="46">
+      <calculatedColumnFormula>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{98D588C0-9131-404A-823E-4F312157B4EE}" name="nombre" dataDxfId="45">
+      <calculatedColumnFormula>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{DA16E63D-3C7B-4235-BC8E-3EB411EC2AF9}" name="nacimiento" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{D65F57BC-8164-4AB7-8337-DE00B9FD8A3A}" name="años" dataDxfId="43">
+      <calculatedColumnFormula array="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{906FCDA3-636B-4283-9205-7AF46F977290}" name="edad" dataDxfId="42" dataCellStyle="Millares">
+      <calculatedColumnFormula>(hoy-datos[[#This Row],[nacimiento]])/365</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{019FA1D5-4F09-4717-AE40-B6C31AA7DC9C}" name="cuil" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{FECB634B-7A6D-4C5C-80DC-9D64C533A46D}" name="g" dataDxfId="40">
+      <calculatedColumnFormula>LEFT(datos[[#This Row],[cuil]],2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{4DAF6AA5-E15E-4B0E-A6B3-0413A3FC7025}" name="docmento" dataDxfId="39">
+      <calculatedColumnFormula>MID(datos[[#This Row],[cuil]],4,8)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{98242B92-44B0-46D8-B255-BEFE9B217C6E}" name="v" dataDxfId="38">
+      <calculatedColumnFormula>RIGHT(datos[[#This Row],[cuil]],1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{96F6AC38-E0D7-4538-BF50-B26B716ECD40}" name="char" dataDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{900EA9DF-7806-4E2A-BE95-A5AA6FF29C93}" name="p" dataDxfId="36">
+      <calculatedColumnFormula>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{7A21E3B8-95EE-4371-95D5-EA3889520837}" name="largo" dataDxfId="35">
+      <calculatedColumnFormula>LEN(datos[[#This Row],[empleado]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}" name="presentismo" displayName="presentismo" ref="A1:AG6" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A1:AG6" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}"/>
   <tableColumns count="33">
     <tableColumn id="1" xr3:uid="{83429F3A-0633-41B4-A217-0D30DFCF116B}" name="Empleado" dataDxfId="32">
       <calculatedColumnFormula>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</calculatedColumnFormula>
@@ -849,25 +1423,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F639E3-C47A-43D0-A8C0-9681F10A43EB}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -881,391 +1464,791 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>33346</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1">
-        <v>34254</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" display="https://www.cuitonline.com/detalle/27452414711/osses-shakira-alejandra.html" xr:uid="{F2232659-C17D-4204-940D-345947882C0E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C54B82-26A3-4EF4-A4EB-E1387A93D0B4}">
+  <dimension ref="A1:V6"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
+        <v>racedo ; cristian Damian</v>
+      </c>
+      <c r="B2" t="str">
+        <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
+        <v xml:space="preserve">racedo </v>
+      </c>
+      <c r="C2" t="str">
+        <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
+        <v>cristian Damian</v>
+      </c>
+      <c r="D2" s="1">
+        <v>33346</v>
+      </c>
+      <c r="E2" s="23" cm="1">
+        <f t="array" aca="1" ref="E2" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <v>31</v>
+      </c>
+      <c r="F2" s="24">
+        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
+        <v>31.646575342465752</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="str">
+        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
+        <v>20</v>
+      </c>
+      <c r="I2" s="6" t="str">
+        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <v>35336446</v>
+      </c>
+      <c r="J2" s="7" t="str">
+        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <v>5</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" s="26">
+        <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
+        <v>8</v>
+      </c>
+      <c r="M2" s="26">
+        <f>LEN(datos[[#This Row],[empleado]])</f>
         <v>24</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="O2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>44897</v>
+      </c>
+      <c r="P2" s="22">
+        <f ca="1">NOW()</f>
+        <v>44897.545370138891</v>
+      </c>
+      <c r="Q2">
+        <f ca="1">YEAR(hoy)</f>
+        <v>2022</v>
+      </c>
+      <c r="R2">
+        <f ca="1">MONTH(hoy)</f>
+        <v>12</v>
+      </c>
+      <c r="S2">
+        <f ca="1">DAY(hoy)</f>
+        <v>2</v>
+      </c>
+      <c r="T2">
+        <f ca="1">HOUR(ahora)</f>
+        <v>13</v>
+      </c>
+      <c r="U2">
+        <f ca="1">MINUTE(ahora)</f>
+        <v>5</v>
+      </c>
+      <c r="V2">
+        <f ca="1">SECOND(ahora)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
+        <v>racedo; Abel Alejandro</v>
+      </c>
+      <c r="B3" t="str">
+        <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
+        <v>racedo</v>
+      </c>
+      <c r="C3" t="str">
+        <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
+        <v>Abel Alejandro</v>
+      </c>
+      <c r="D3" s="1">
+        <v>34254</v>
+      </c>
+      <c r="E3" s="23" cm="1">
+        <f t="array" aca="1" ref="E3" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <v>29</v>
+      </c>
+      <c r="F3" s="24">
+        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
+        <v>29.158904109589042</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="8" t="str">
+        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
+        <v>20</v>
+      </c>
+      <c r="I3" s="8" t="str">
+        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <v>38558443</v>
+      </c>
+      <c r="J3" s="9" t="str">
+        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <v>6</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="L3" s="27">
+        <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
+        <v>7</v>
+      </c>
+      <c r="M3" s="27">
+        <f>LEN(datos[[#This Row],[empleado]])</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
+        <v>Aguilera; Cristina</v>
+      </c>
+      <c r="B4" t="str">
+        <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
+        <v>Aguilera</v>
+      </c>
+      <c r="C4" t="str">
+        <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
+        <v>Cristina</v>
+      </c>
+      <c r="D4" s="1">
         <v>29573</v>
       </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="E4" s="23" cm="1">
+        <f t="array" aca="1" ref="E4" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <v>42</v>
+      </c>
+      <c r="F4" s="24">
+        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
+        <v>41.983561643835614</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="6" t="str">
+        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
         <v>27</v>
+      </c>
+      <c r="I4" s="6" t="str">
+        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <v>14093915</v>
+      </c>
+      <c r="J4" s="7" t="str">
+        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <v>9</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="L4" s="26">
+        <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
+        <v>9</v>
+      </c>
+      <c r="M4" s="26">
+        <f>LEN(datos[[#This Row],[empleado]])</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
+        <v>Osses; Shakira Alejandra</v>
+      </c>
+      <c r="B5" t="str">
+        <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
+        <v>Osses</v>
+      </c>
+      <c r="C5" t="str">
+        <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
+        <v>Shakira Alejandra</v>
+      </c>
+      <c r="D5" s="1">
+        <v>28158</v>
+      </c>
+      <c r="E5" s="23" cm="1">
+        <f t="array" aca="1" ref="E5" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <v>45</v>
+      </c>
+      <c r="F5" s="24">
+        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
+        <v>45.860273972602741</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="8" t="str">
+        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
+        <v>27</v>
+      </c>
+      <c r="I5" s="8" t="str">
+        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <v>45241471</v>
+      </c>
+      <c r="J5" s="9" t="str">
+        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="27">
+        <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
+        <v>6</v>
+      </c>
+      <c r="M5" s="27">
+        <f>LEN(datos[[#This Row],[empleado]])</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
+        <v>Messi ; Lionel Andres</v>
+      </c>
+      <c r="B6" t="str">
+        <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
+        <v xml:space="preserve">Messi </v>
+      </c>
+      <c r="C6" t="str">
+        <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
+        <v>Lionel Andres</v>
+      </c>
+      <c r="D6" s="1">
+        <v>31952</v>
+      </c>
+      <c r="E6" s="23" cm="1">
+        <f t="array" aca="1" ref="E6" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <v>35</v>
+      </c>
+      <c r="F6" s="24">
+        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
+        <v>35.465753424657535</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="6" t="str">
+        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
+        <v>23</v>
+      </c>
+      <c r="I6" s="6" t="str">
+        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <v>33016244</v>
+      </c>
+      <c r="J6" s="7" t="str">
+        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <v>9</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" s="26">
+        <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
+        <v>7</v>
+      </c>
+      <c r="M6" s="26">
+        <f>LEN(datos[[#This Row],[empleado]])</f>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FFAE78-438E-4183-90FE-F9F4BDD2CD47}">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH2" sqref="AH2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="3.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="3.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="3.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="3.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="3.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.42578125" style="5" customWidth="1"/>
-    <col min="32" max="32" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="20" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.42578125" style="11" customWidth="1"/>
+    <col min="32" max="32" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="G1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="I1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="J1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="K1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="L1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="M1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="N1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="O1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="P1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="Q1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="R1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="S1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="T1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="U1" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="V1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="W1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="X1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="Y1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="Z1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="AA1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="AB1" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="AC1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="AD1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AE1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AF1" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AG1" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AI1" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AJ1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK1" t="s">
         <v>57</v>
       </c>
-      <c r="AD1" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="str">
+      <c r="A2" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
-        <v>racedo; cristian</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="U2" s="9"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF2" s="12">
+        <v>racedo    ; cristian Damian</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="15"/>
+      <c r="O2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="15"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF2" s="18">
         <f>COUNTA(B2:AE2)</f>
         <v>19</v>
       </c>
-      <c r="AG2" s="12">
+      <c r="AG2" s="18">
         <f>COUNTBLANK(B2:AE2)</f>
         <v>11</v>
       </c>
       <c r="AI2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AJ2">
         <f>SUM(presentismo[ASIST])</f>
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="AK2">
         <f>SUM(presentismo[AUS])</f>
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="str">
+      <c r="A3" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
-        <v>racedo; abel</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF3" s="12">
-        <f t="shared" ref="AF2:AF4" si="0">COUNTA(B3:AE3)</f>
+        <v xml:space="preserve">    racedo; Abel      Alejandro</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF3" s="18">
+        <f t="shared" ref="AF3:AF4" si="0">COUNTA(B3:AE3)</f>
         <v>16</v>
       </c>
-      <c r="AG3" s="12">
-        <f t="shared" ref="AG2:AG4" si="1">COUNTBLANK(B3:AE3)</f>
+      <c r="AG3" s="18">
+        <f t="shared" ref="AG3:AG4" si="1">COUNTBLANK(B3:AE3)</f>
         <v>14</v>
       </c>
       <c r="AI3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="AJ3">
         <f>MAX(presentismo[ASIST])</f>
@@ -1277,75 +2260,79 @@
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="str">
+      <c r="A4" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
-        <v>Aguilera; Cristina</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="X4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF4" s="12">
+        <v xml:space="preserve">   Aguilera; Cristina     </v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="X4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF4" s="18">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AG4" s="12">
+        <v>19</v>
+      </c>
+      <c r="AG4" s="18">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AI4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="AJ4">
         <f>MIN(presentismo[ASIST])</f>
@@ -1357,23 +2344,155 @@
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
+      <c r="A5" s="17" t="str">
+        <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
+        <v>Osses; Shakira      Alejandra</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="W5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="X5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF5" s="18">
+        <f t="shared" ref="AF5:AF6" si="2">COUNTA(B5:AE5)</f>
+        <v>16</v>
+      </c>
+      <c r="AG5" s="18">
+        <f t="shared" ref="AG5" si="3">COUNTBLANK(B5:AE5)</f>
+        <v>14</v>
+      </c>
       <c r="AI5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ5" s="13">
+        <v>61</v>
+      </c>
+      <c r="AJ5" s="19">
         <f>AVERAGE(presentismo[ASIST])</f>
-        <v>17.666666666666668</v>
-      </c>
-      <c r="AK5" s="13">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="AK5" s="19">
         <f>AVERAGE(presentismo[AUS])</f>
-        <v>12.333333333333334</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
+      <c r="A6" s="17" t="str">
+        <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
+        <v xml:space="preserve">Messi    ; Lionel      Andres </v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="11"/>
+      <c r="I6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="W6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="X6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF6" s="18">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="AG6" s="18">
+        <f>COUNTBLANK(B6:AE6)</f>
+        <v>12</v>
+      </c>
       <c r="AI6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="AJ6">
         <f>MEDIAN(presentismo[ASIST])</f>
@@ -1385,90 +2504,90 @@
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+      <c r="B7" s="14"/>
       <c r="AI7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AJ7" t="e">
+        <v>63</v>
+      </c>
+      <c r="AJ7">
         <f>MODE(presentismo[ASIST])</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AK7" t="e">
+        <v>19</v>
+      </c>
+      <c r="AK7">
         <f>MODE(presentismo[AUS])</f>
-        <v>#N/A</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+      <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
+      <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
+      <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
+      <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
+      <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
+      <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
+      <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="B16" s="14"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+      <c r="B17" s="14"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
+      <c r="B18" s="14"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
+      <c r="B19" s="14"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
+      <c r="B20" s="14"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
+      <c r="B21" s="14"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
+      <c r="B22" s="14"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
+      <c r="B23" s="14"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
+      <c r="B24" s="14"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
+      <c r="B25" s="14"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
+      <c r="B26" s="14"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
+      <c r="B27" s="14"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
+      <c r="B28" s="14"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
+      <c r="B29" s="14"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
+      <c r="B30" s="14"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
+      <c r="B31" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1478,7 +2597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BCF59A-9D0C-4ADD-8102-A58A6DC81599}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1490,7 +2609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3FF01-9040-4806-AC6E-6DE86411CAF8}">
   <dimension ref="A1:J11"/>
   <sheetViews>
@@ -1513,28 +2632,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="J1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1554,15 +2673,15 @@
         <v>15000</v>
       </c>
       <c r="F2" s="3">
-        <f>cant*precio</f>
+        <f t="shared" ref="F2:F11" si="0">cant*precio</f>
         <v>30000</v>
       </c>
       <c r="G2" s="3">
-        <f>total*iva</f>
+        <f t="shared" ref="G2:G11" si="1">total*iva</f>
         <v>6300</v>
       </c>
       <c r="H2" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" ref="H2:H11" si="2">total +precio_iva</f>
         <v>36300</v>
       </c>
       <c r="J2" s="2">
@@ -1586,15 +2705,15 @@
         <v>5400</v>
       </c>
       <c r="F3" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>21600</v>
       </c>
       <c r="G3" s="3">
-        <f>total*iva</f>
+        <f t="shared" si="1"/>
         <v>4536</v>
       </c>
       <c r="H3" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" si="2"/>
         <v>26136</v>
       </c>
     </row>
@@ -1615,15 +2734,15 @@
         <v>3800</v>
       </c>
       <c r="F4" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>11400</v>
       </c>
       <c r="G4" s="3">
-        <f>total*iva</f>
+        <f t="shared" si="1"/>
         <v>2394</v>
       </c>
       <c r="H4" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" si="2"/>
         <v>13794</v>
       </c>
     </row>
@@ -1644,15 +2763,15 @@
         <v>600</v>
       </c>
       <c r="F5" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="G5" s="3">
-        <f>total*iva</f>
+        <f t="shared" si="1"/>
         <v>126</v>
       </c>
       <c r="H5" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" si="2"/>
         <v>726</v>
       </c>
     </row>
@@ -1673,15 +2792,15 @@
         <v>8800</v>
       </c>
       <c r="F6" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>52800</v>
       </c>
       <c r="G6" s="3">
-        <f>total*iva</f>
+        <f t="shared" si="1"/>
         <v>11088</v>
       </c>
       <c r="H6" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" si="2"/>
         <v>63888</v>
       </c>
     </row>
@@ -1702,15 +2821,15 @@
         <v>8800</v>
       </c>
       <c r="F7" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>88000</v>
       </c>
       <c r="G7" s="3">
-        <f>total*iva</f>
+        <f t="shared" si="1"/>
         <v>18480</v>
       </c>
       <c r="H7" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" si="2"/>
         <v>106480</v>
       </c>
     </row>
@@ -1731,15 +2850,15 @@
         <v>600</v>
       </c>
       <c r="F8" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>18000</v>
       </c>
       <c r="G8" s="3">
-        <f>total*iva</f>
+        <f t="shared" si="1"/>
         <v>3780</v>
       </c>
       <c r="H8" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" si="2"/>
         <v>21780</v>
       </c>
     </row>
@@ -1760,15 +2879,15 @@
         <v>3800</v>
       </c>
       <c r="F9" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>7600</v>
       </c>
       <c r="G9" s="3">
-        <f>total*iva</f>
+        <f t="shared" si="1"/>
         <v>1596</v>
       </c>
       <c r="H9" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" si="2"/>
         <v>9196</v>
       </c>
     </row>
@@ -1789,15 +2908,15 @@
         <v>15000</v>
       </c>
       <c r="F10" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
       <c r="G10" s="3">
-        <f>total*iva</f>
+        <f t="shared" si="1"/>
         <v>3150</v>
       </c>
       <c r="H10" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" si="2"/>
         <v>18150</v>
       </c>
     </row>
@@ -1818,15 +2937,15 @@
         <v>3800</v>
       </c>
       <c r="F11" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>7600</v>
       </c>
       <c r="G11" s="3">
-        <f>total*iva</f>
+        <f t="shared" si="1"/>
         <v>1596</v>
       </c>
       <c r="H11" s="3">
-        <f>total +precio_iva</f>
+        <f t="shared" si="2"/>
         <v>9196</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Funciones de Texto MAYUSC
</commit_message>
<xml_diff>
--- a/empresa.xlsx
+++ b/empresa.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xls-v10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9B1A19-643B-4089-B1C5-499A7D73E950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2AF0E7-113B-45BD-90D1-632D1485B0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBF13C54-EAF5-48F7-B675-6702B08EF7EF}"/>
   </bookViews>
   <sheets>
-    <sheet name="empleados" sheetId="1" r:id="rId1"/>
-    <sheet name="datos" sheetId="5" r:id="rId2"/>
-    <sheet name="presentismo" sheetId="4" r:id="rId3"/>
-    <sheet name="productos" sheetId="2" r:id="rId4"/>
-    <sheet name="ventas" sheetId="3" r:id="rId5"/>
+    <sheet name="menu" sheetId="6" r:id="rId1"/>
+    <sheet name="empleados" sheetId="1" r:id="rId2"/>
+    <sheet name="datos" sheetId="5" r:id="rId3"/>
+    <sheet name="presentismo" sheetId="4" r:id="rId4"/>
+    <sheet name="productos" sheetId="2" r:id="rId5"/>
+    <sheet name="ventas" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="ahora">datos!$P$2</definedName>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -70,29 +71,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="108">
   <si>
     <t>codigo</t>
   </si>
   <si>
-    <t>apellido</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>legajo</t>
-  </si>
-  <si>
-    <t>edad</t>
-  </si>
-  <si>
-    <t>sector</t>
-  </si>
-  <si>
-    <t>cuil</t>
-  </si>
-  <si>
     <t>cdr18491</t>
   </si>
   <si>
@@ -303,12 +286,6 @@
     <t>DIA</t>
   </si>
   <si>
-    <t>años</t>
-  </si>
-  <si>
-    <t>nacimiento</t>
-  </si>
-  <si>
     <t>HH</t>
   </si>
   <si>
@@ -318,15 +295,6 @@
     <t>ss</t>
   </si>
   <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>docmento</t>
-  </si>
-  <si>
     <t>empleado</t>
   </si>
   <si>
@@ -342,28 +310,91 @@
     <t>cristian Damian</t>
   </si>
   <si>
-    <t xml:space="preserve">racedo    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    racedo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Aguilera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cristina     </t>
-  </si>
-  <si>
-    <t>Abel      Alejandro</t>
-  </si>
-  <si>
-    <t>Shakira      Alejandra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lionel      Andres </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Messi    </t>
+    <t>racedo</t>
+  </si>
+  <si>
+    <t>Abel Alejandro</t>
+  </si>
+  <si>
+    <t>Aguilera</t>
+  </si>
+  <si>
+    <t>Cristina</t>
+  </si>
+  <si>
+    <t>Shakira Alejandra</t>
+  </si>
+  <si>
+    <t>Messi</t>
+  </si>
+  <si>
+    <t>Lionel Andres</t>
+  </si>
+  <si>
+    <t>CODIGO</t>
+  </si>
+  <si>
+    <t>APELLIDO</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>LEGAJO</t>
+  </si>
+  <si>
+    <t>SECTOR</t>
+  </si>
+  <si>
+    <t>NACIMIENTO</t>
+  </si>
+  <si>
+    <t>AÑOS</t>
+  </si>
+  <si>
+    <t>EDAD</t>
+  </si>
+  <si>
+    <t>CUIL</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>DOCMENTO</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Empleados</t>
+  </si>
+  <si>
+    <t>Datos</t>
+  </si>
+  <si>
+    <t>Asistencia</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t>Nuevo</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>Atajos</t>
+  </si>
+  <si>
+    <t>Alumni</t>
+  </si>
+  <si>
+    <t>GitHub</t>
   </si>
 </sst>
 </file>
@@ -993,11 +1024,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}" name="empleados" displayName="empleados" ref="A1:E6" totalsRowShown="0">
   <autoFilter ref="A1:E6" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9B2FABCB-122E-4021-BCB9-1ABCF38F08D1}" name="codigo"/>
-    <tableColumn id="2" xr3:uid="{48BCCCB0-2E0A-4212-A44B-A72FF9EFADA4}" name="apellido"/>
-    <tableColumn id="3" xr3:uid="{8E2D81A4-6B1C-4EE6-B057-EC49A27E5F85}" name="nombre"/>
-    <tableColumn id="4" xr3:uid="{FAD0BCDF-63FA-416C-A9FA-7BBA19E4DC2A}" name="legajo"/>
-    <tableColumn id="7" xr3:uid="{B0450268-4DC5-4E02-B6A4-0DBA5EAA50A9}" name="sector"/>
+    <tableColumn id="1" xr3:uid="{9B2FABCB-122E-4021-BCB9-1ABCF38F08D1}" name="CODIGO"/>
+    <tableColumn id="2" xr3:uid="{48BCCCB0-2E0A-4212-A44B-A72FF9EFADA4}" name="APELLIDO"/>
+    <tableColumn id="3" xr3:uid="{8E2D81A4-6B1C-4EE6-B057-EC49A27E5F85}" name="NOMBRE"/>
+    <tableColumn id="4" xr3:uid="{FAD0BCDF-63FA-416C-A9FA-7BBA19E4DC2A}" name="LEGAJO"/>
+    <tableColumn id="7" xr3:uid="{B0450268-4DC5-4E02-B6A4-0DBA5EAA50A9}" name="SECTOR"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1043,28 +1074,28 @@
     <tableColumn id="1" xr3:uid="{1E40E760-3B7A-46CB-ADE6-9C36221D8FBE}" name="empleado" dataDxfId="47">
       <calculatedColumnFormula>TRIM(presentismo[[#This Row],[Empleado]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A673056C-D666-4A82-8F15-DA591ECD51CD}" name="apellido" dataDxfId="46">
+    <tableColumn id="2" xr3:uid="{A673056C-D666-4A82-8F15-DA591ECD51CD}" name="APELLIDO" dataDxfId="46">
       <calculatedColumnFormula>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{98D588C0-9131-404A-823E-4F312157B4EE}" name="nombre" dataDxfId="45">
+    <tableColumn id="3" xr3:uid="{98D588C0-9131-404A-823E-4F312157B4EE}" name="NOMBRE" dataDxfId="45">
       <calculatedColumnFormula>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DA16E63D-3C7B-4235-BC8E-3EB411EC2AF9}" name="nacimiento" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{D65F57BC-8164-4AB7-8337-DE00B9FD8A3A}" name="años" dataDxfId="43">
-      <calculatedColumnFormula array="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{DA16E63D-3C7B-4235-BC8E-3EB411EC2AF9}" name="NACIMIENTO" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{D65F57BC-8164-4AB7-8337-DE00B9FD8A3A}" name="AÑOS" dataDxfId="43">
+      <calculatedColumnFormula array="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{906FCDA3-636B-4283-9205-7AF46F977290}" name="edad" dataDxfId="42" dataCellStyle="Millares">
-      <calculatedColumnFormula>(hoy-datos[[#This Row],[nacimiento]])/365</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{906FCDA3-636B-4283-9205-7AF46F977290}" name="EDAD" dataDxfId="42" dataCellStyle="Millares">
+      <calculatedColumnFormula>(hoy-datos[[#This Row],[NACIMIENTO]])/365</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{019FA1D5-4F09-4717-AE40-B6C31AA7DC9C}" name="cuil" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{FECB634B-7A6D-4C5C-80DC-9D64C533A46D}" name="g" dataDxfId="40">
-      <calculatedColumnFormula>LEFT(datos[[#This Row],[cuil]],2)</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{019FA1D5-4F09-4717-AE40-B6C31AA7DC9C}" name="CUIL" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{FECB634B-7A6D-4C5C-80DC-9D64C533A46D}" name="G" dataDxfId="40">
+      <calculatedColumnFormula>LEFT(datos[[#This Row],[CUIL]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4DAF6AA5-E15E-4B0E-A6B3-0413A3FC7025}" name="docmento" dataDxfId="39">
-      <calculatedColumnFormula>MID(datos[[#This Row],[cuil]],4,8)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{4DAF6AA5-E15E-4B0E-A6B3-0413A3FC7025}" name="DOCMENTO" dataDxfId="39">
+      <calculatedColumnFormula>MID(datos[[#This Row],[CUIL]],4,8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{98242B92-44B0-46D8-B255-BEFE9B217C6E}" name="v" dataDxfId="38">
-      <calculatedColumnFormula>RIGHT(datos[[#This Row],[cuil]],1)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{98242B92-44B0-46D8-B255-BEFE9B217C6E}" name="V" dataDxfId="38">
+      <calculatedColumnFormula>RIGHT(datos[[#This Row],[CUIL]],1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{96F6AC38-E0D7-4538-BF50-B26B716ECD40}" name="char" dataDxfId="37"/>
     <tableColumn id="12" xr3:uid="{900EA9DF-7806-4E2A-BE95-A5AA6FF29C93}" name="p" dataDxfId="36">
@@ -1083,7 +1114,7 @@
   <autoFilter ref="A1:AG6" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}"/>
   <tableColumns count="33">
     <tableColumn id="1" xr3:uid="{83429F3A-0633-41B4-A217-0D30DFCF116B}" name="Empleado" dataDxfId="32">
-      <calculatedColumnFormula>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{887EC86C-1521-40B0-A6C3-0B2B3230C024}" name="1/11/22" dataDxfId="31"/>
     <tableColumn id="3" xr3:uid="{C8618297-DB24-4382-BD1E-E53E7DB10A63}" name="2/11/22" dataDxfId="30"/>
@@ -1422,10 +1453,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBB5BBC-F064-4678-AF8C-C3D428764205}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F639E3-C47A-43D0-A8C0-9681F10A43EB}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1436,13 +1518,13 @@
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
@@ -1452,19 +1534,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1472,16 +1554,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1489,16 +1571,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1506,16 +1588,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F4" s="10"/>
     </row>
@@ -1524,16 +1606,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1541,16 +1623,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1566,103 +1648,104 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C54B82-26A3-4EF4-A4EB-E1387A93D0B4}">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J8" sqref="B8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="0.28515625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="3.42578125" customWidth="1"/>
+    <col min="11" max="11" width="0.28515625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="25" t="s">
+      <c r="O1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" t="s">
         <v>72</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>73</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>74</v>
-      </c>
-      <c r="R1" t="s">
-        <v>75</v>
-      </c>
-      <c r="S1" t="s">
-        <v>76</v>
-      </c>
-      <c r="T1" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
-        <v>racedo ; cristian Damian</v>
+        <v>racedo; cristian Damian</v>
       </c>
       <c r="B2" t="str">
         <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
-        <v xml:space="preserve">racedo </v>
+        <v>racedo</v>
       </c>
       <c r="C2" t="str">
         <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
@@ -1672,46 +1755,46 @@
         <v>33346</v>
       </c>
       <c r="E2" s="23" cm="1">
-        <f t="array" aca="1" ref="E2" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <f t="array" aca="1" ref="E2" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>31</v>
       </c>
       <c r="F2" s="24">
-        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
-        <v>31.646575342465752</v>
+        <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
+        <v>31.684931506849313</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H2" s="6" t="str">
-        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
+        <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>20</v>
       </c>
       <c r="I2" s="6" t="str">
-        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>35336446</v>
       </c>
       <c r="J2" s="7" t="str">
-        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>5</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="L2" s="26">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M2" s="26">
         <f>LEN(datos[[#This Row],[empleado]])</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44897</v>
+        <v>44911</v>
       </c>
       <c r="P2" s="22">
         <f ca="1">NOW()</f>
-        <v>44897.545370138891</v>
+        <v>44911.428219675923</v>
       </c>
       <c r="Q2">
         <f ca="1">YEAR(hoy)</f>
@@ -1723,19 +1806,19 @@
       </c>
       <c r="S2">
         <f ca="1">DAY(hoy)</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="T2">
         <f ca="1">HOUR(ahora)</f>
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="U2">
         <f ca="1">MINUTE(ahora)</f>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="V2">
         <f ca="1">SECOND(ahora)</f>
-        <v>20</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1755,30 +1838,30 @@
         <v>34254</v>
       </c>
       <c r="E3" s="23" cm="1">
-        <f t="array" aca="1" ref="E3" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <f t="array" aca="1" ref="E3" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>29</v>
       </c>
       <c r="F3" s="24">
-        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
-        <v>29.158904109589042</v>
+        <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
+        <v>29.197260273972603</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H3" s="8" t="str">
-        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
+        <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>20</v>
       </c>
       <c r="I3" s="8" t="str">
-        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>38558443</v>
       </c>
       <c r="J3" s="9" t="str">
-        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>6</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="L3" s="27">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
@@ -1806,30 +1889,30 @@
         <v>29573</v>
       </c>
       <c r="E4" s="23" cm="1">
-        <f t="array" aca="1" ref="E4" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <f t="array" aca="1" ref="E4" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>42</v>
       </c>
       <c r="F4" s="24">
-        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
-        <v>41.983561643835614</v>
+        <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
+        <v>42.021917808219179</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H4" s="6" t="str">
-        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
+        <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>27</v>
       </c>
       <c r="I4" s="6" t="str">
-        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>14093915</v>
       </c>
       <c r="J4" s="7" t="str">
-        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>9</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="L4" s="26">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
@@ -1857,30 +1940,30 @@
         <v>28158</v>
       </c>
       <c r="E5" s="23" cm="1">
-        <f t="array" aca="1" ref="E5" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <f t="array" aca="1" ref="E5" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>45</v>
       </c>
       <c r="F5" s="24">
-        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
-        <v>45.860273972602741</v>
+        <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
+        <v>45.898630136986299</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H5" s="8" t="str">
-        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
+        <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>27</v>
       </c>
       <c r="I5" s="8" t="str">
-        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>45241471</v>
       </c>
       <c r="J5" s="9" t="str">
-        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>1</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="L5" s="27">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
@@ -1894,11 +1977,11 @@
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
-        <v>Messi ; Lionel Andres</v>
+        <v>Messi; Lionel Andres</v>
       </c>
       <c r="B6" t="str">
         <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
-        <v xml:space="preserve">Messi </v>
+        <v>Messi</v>
       </c>
       <c r="C6" t="str">
         <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
@@ -1908,38 +1991,38 @@
         <v>31952</v>
       </c>
       <c r="E6" s="23" cm="1">
-        <f t="array" aca="1" ref="E6" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[nacimiento]])</f>
+        <f t="array" aca="1" ref="E6" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>35</v>
       </c>
       <c r="F6" s="24">
-        <f ca="1">(hoy-datos[[#This Row],[nacimiento]])/365</f>
-        <v>35.465753424657535</v>
+        <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
+        <v>35.504109589041093</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H6" s="6" t="str">
-        <f>LEFT(datos[[#This Row],[cuil]],2)</f>
+        <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>23</v>
       </c>
       <c r="I6" s="6" t="str">
-        <f>MID(datos[[#This Row],[cuil]],4,8)</f>
+        <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>33016244</v>
       </c>
       <c r="J6" s="7" t="str">
-        <f>RIGHT(datos[[#This Row],[cuil]],1)</f>
+        <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>9</v>
       </c>
       <c r="K6" s="26" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="L6" s="26">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M6" s="26">
         <f>LEN(datos[[#This Row],[empleado]])</f>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1951,15 +2034,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FFAE78-438E-4183-90FE-F9F4BDD2CD47}">
   <dimension ref="A1:AK31"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1981,186 +2064,186 @@
   <sheetData>
     <row r="1" spans="1:37" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="G1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="N1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="T1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="U1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="V1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="AA1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="AB1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="AC1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="AD1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="AE1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AF1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AG1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AI1" t="s">
         <v>50</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AJ1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" t="s">
         <v>51</v>
-      </c>
-      <c r="AD1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AF1" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG1" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="str">
-        <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
-        <v>racedo    ; cristian Damian</v>
+        <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
+        <v>racedo; cristian Damian</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K2" s="14"/>
       <c r="L2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N2" s="15"/>
       <c r="O2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="P2" s="14"/>
       <c r="Q2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="R2" s="14"/>
       <c r="S2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="U2" s="15"/>
       <c r="V2" s="14"/>
       <c r="W2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="X2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Y2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Z2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AA2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AB2" s="15"/>
       <c r="AC2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AD2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AE2" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AF2" s="18">
         <f>COUNTA(B2:AE2)</f>
@@ -2171,7 +2254,7 @@
         <v>11</v>
       </c>
       <c r="AI2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="AJ2">
         <f>SUM(presentismo[ASIST])</f>
@@ -2184,60 +2267,60 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="str">
-        <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
-        <v xml:space="preserve">    racedo; Abel      Alejandro</v>
+        <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
+        <v>racedo; Abel Alejandro</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="R3" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="V3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="X3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Y3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Z3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AF3" s="18">
         <f t="shared" ref="AF3:AF4" si="0">COUNTA(B3:AE3)</f>
@@ -2248,7 +2331,7 @@
         <v>14</v>
       </c>
       <c r="AI3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="AJ3">
         <f>MAX(presentismo[ASIST])</f>
@@ -2261,67 +2344,67 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="str">
-        <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
-        <v xml:space="preserve">   Aguilera; Cristina     </v>
+        <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
+        <v>Aguilera; Cristina</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N4" s="11"/>
       <c r="O4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="S4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="X4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Y4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Z4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AA4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AD4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AE4" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AF4" s="18">
         <f t="shared" si="0"/>
@@ -2332,7 +2415,7 @@
         <v>11</v>
       </c>
       <c r="AI4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AJ4">
         <f>MIN(presentismo[ASIST])</f>
@@ -2345,60 +2428,60 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="str">
-        <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
-        <v>Osses; Shakira      Alejandra</v>
+        <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
+        <v>Osses; Shakira Alejandra</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N5" s="11"/>
       <c r="O5" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="T5" s="14"/>
       <c r="U5" s="14"/>
       <c r="V5" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="W5" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="AA5" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AD5" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AE5" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AF5" s="18">
         <f t="shared" ref="AF5:AF6" si="2">COUNTA(B5:AE5)</f>
@@ -2409,7 +2492,7 @@
         <v>14</v>
       </c>
       <c r="AI5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="AJ5" s="19">
         <f>AVERAGE(presentismo[ASIST])</f>
@@ -2422,66 +2505,66 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="str">
-        <f>_xlfn.CONCAT(empleados[[#This Row],[apellido]]&amp;"; "&amp;empleados[[#This Row],[nombre]])</f>
-        <v xml:space="preserve">Messi    ; Lionel      Andres </v>
+        <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
+        <v>Messi; Lionel Andres</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N6" s="11"/>
       <c r="O6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="U6" s="11"/>
       <c r="V6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="W6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="X6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Z6" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AA6" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AC6" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AD6" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="AF6" s="18">
         <f t="shared" si="2"/>
@@ -2492,7 +2575,7 @@
         <v>12</v>
       </c>
       <c r="AI6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="AJ6">
         <f>MEDIAN(presentismo[ASIST])</f>
@@ -2506,7 +2589,7 @@
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="AI7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="AJ7">
         <f>MODE(presentismo[ASIST])</f>
@@ -2597,7 +2680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BCF59A-9D0C-4ADD-8102-A58A6DC81599}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2609,12 +2692,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3FF01-9040-4806-AC6E-6DE86411CAF8}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2632,28 +2715,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2681,7 +2764,7 @@
         <v>6300</v>
       </c>
       <c r="H2" s="3">
-        <f t="shared" ref="H2:H11" si="2">total +precio_iva</f>
+        <f>total +precio_iva</f>
         <v>36300</v>
       </c>
       <c r="J2" s="2">
@@ -2713,7 +2796,7 @@
         <v>4536</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H2:H11" si="2">total +precio_iva</f>
         <v>26136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hipervinculos Internos y Externos
</commit_message>
<xml_diff>
--- a/empresa.xlsx
+++ b/empresa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xls-v10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2AF0E7-113B-45BD-90D1-632D1485B0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944B5502-3280-4E85-8484-0B17BA5C9AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBF13C54-EAF5-48F7-B675-6702B08EF7EF}"/>
   </bookViews>
@@ -19,16 +19,17 @@
     <sheet name="presentismo" sheetId="4" r:id="rId4"/>
     <sheet name="productos" sheetId="2" r:id="rId5"/>
     <sheet name="ventas" sheetId="3" r:id="rId6"/>
+    <sheet name="estadisticas" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="ahora">datos!$P$2</definedName>
-    <definedName name="año">datos!$Q$2</definedName>
-    <definedName name="cant">ventas!$D:$D</definedName>
-    <definedName name="hoy">datos!$O$2</definedName>
-    <definedName name="iva">ventas!$J$2</definedName>
-    <definedName name="precio">ventas!$E:$E</definedName>
-    <definedName name="precio_iva">ventas!$G:$G</definedName>
-    <definedName name="total">ventas!$F:$F</definedName>
+    <definedName name="ahora">datos!$Q$2</definedName>
+    <definedName name="año">datos!$R$2</definedName>
+    <definedName name="cant">ventas!$E:$E</definedName>
+    <definedName name="hoy">datos!$P$2</definedName>
+    <definedName name="iva">ventas!$K$2</definedName>
+    <definedName name="precio">ventas!$F:$F</definedName>
+    <definedName name="precio_iva">ventas!$H:$H</definedName>
+    <definedName name="total">ventas!$G:$G</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="112">
   <si>
     <t>codigo</t>
   </si>
@@ -395,6 +396,18 @@
   </si>
   <si>
     <t>GitHub</t>
+  </si>
+  <si>
+    <t>Internos</t>
+  </si>
+  <si>
+    <t>Externos</t>
+  </si>
+  <si>
+    <t>atras</t>
+  </si>
+  <si>
+    <t>Intro</t>
   </si>
 </sst>
 </file>
@@ -408,7 +421,7 @@
     <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,8 +478,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,6 +511,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,13 +552,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -574,8 +608,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Énfasis1" xfId="4" builtinId="29"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1021,8 +1076,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}" name="empleados" displayName="empleados" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}" name="empleados" displayName="empleados" ref="B1:F6" totalsRowShown="0">
+  <autoFilter ref="B1:F6" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{9B2FABCB-122E-4021-BCB9-1ABCF38F08D1}" name="CODIGO"/>
     <tableColumn id="2" xr3:uid="{48BCCCB0-2E0A-4212-A44B-A72FF9EFADA4}" name="APELLIDO"/>
@@ -1035,8 +1090,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{21CB7767-E429-4D32-8B4C-B110EB0BC09A}" name="tiempo" displayName="tiempo" ref="O1:V2" totalsRowShown="0">
-  <autoFilter ref="O1:V2" xr:uid="{21CB7767-E429-4D32-8B4C-B110EB0BC09A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{21CB7767-E429-4D32-8B4C-B110EB0BC09A}" name="tiempo" displayName="tiempo" ref="P1:W2" totalsRowShown="0">
+  <autoFilter ref="P1:W2" xr:uid="{21CB7767-E429-4D32-8B4C-B110EB0BC09A}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D0C157DB-5866-4540-85DA-CA9246E3491C}" name="HOY" dataDxfId="51">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
@@ -1068,8 +1123,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A8CA9039-9259-406D-B167-9DC94801EDAB}" name="datos" displayName="datos" ref="A1:M6" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
-  <autoFilter ref="A1:M6" xr:uid="{A8CA9039-9259-406D-B167-9DC94801EDAB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A8CA9039-9259-406D-B167-9DC94801EDAB}" name="datos" displayName="datos" ref="B1:N6" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
+  <autoFilter ref="B1:N6" xr:uid="{A8CA9039-9259-406D-B167-9DC94801EDAB}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{1E40E760-3B7A-46CB-ADE6-9C36221D8FBE}" name="empleado" dataDxfId="47">
       <calculatedColumnFormula>TRIM(presentismo[[#This Row],[Empleado]])</calculatedColumnFormula>
@@ -1110,8 +1165,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}" name="presentismo" displayName="presentismo" ref="A1:AG6" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A1:AG6" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}" name="presentismo" displayName="presentismo" ref="B1:AH6" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="B1:AH6" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}"/>
   <tableColumns count="33">
     <tableColumn id="1" xr3:uid="{83429F3A-0633-41B4-A217-0D30DFCF116B}" name="Empleado" dataDxfId="32">
       <calculatedColumnFormula>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</calculatedColumnFormula>
@@ -1147,10 +1202,10 @@
     <tableColumn id="30" xr3:uid="{6FCC3D91-E530-49DC-9803-12984CBA6BE9}" name="29/11/22" dataDxfId="3"/>
     <tableColumn id="31" xr3:uid="{E6DAAE99-A983-4374-B5B5-FA292704266A}" name="30/11/22" dataDxfId="2"/>
     <tableColumn id="32" xr3:uid="{9612EC83-2684-4EAF-A263-5FD181F5472E}" name="ASIST" dataDxfId="1">
-      <calculatedColumnFormula>COUNTA(B2:AE2)</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTA(C2:AF2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{CF4CC9FE-4916-47D6-BF2F-CC31868C00D4}" name="AUS" dataDxfId="0">
-      <calculatedColumnFormula>COUNTBLANK(B2:AE2)</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTBLANK(C2:AF2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1454,191 +1509,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBB5BBC-F064-4678-AF8C-C3D428764205}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="35" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="G2" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" s="35" t="s">
         <v>107</v>
       </c>
+      <c r="H4" s="29"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="H3:H4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" location="empleados!A1" display="Empleados" xr:uid="{6804FC27-9203-4DBA-8D6C-376C27FE298D}"/>
+    <hyperlink ref="C2" location="datos!A1" display="Datos" xr:uid="{95B4B2CA-F76F-4EDE-AD89-FABD1945827F}"/>
+    <hyperlink ref="D2" location="presentismo!A1" display="Asistencia" xr:uid="{721BE012-66AF-40FB-8AA4-88D83F8A65DF}"/>
+    <hyperlink ref="E2" location="productos!A1" display="Productos" xr:uid="{879548AE-FA71-43F2-A80B-9451463218EE}"/>
+    <hyperlink ref="F2" location="ventas!A1" display="Ventas" xr:uid="{6E77832F-4432-4CDA-92E6-41CCFC5503FD}"/>
+    <hyperlink ref="G2" location="estadisticas!A1" display="Estadisticas" xr:uid="{7EA053B9-79E3-4EA2-901A-779E743F5AFC}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{469E7BDF-AAAE-4702-AFCD-1FFC79427B87}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{580195E5-4F03-40CD-BE17-C7D722BA18BB}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{FFEBE6DB-262E-4357-8099-4D0AA8A0BE5A}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{EFA6FED0-2644-4928-8B05-19C80BA7BDEB}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{9512EF5E-D632-428D-889F-850ADAE7EC32}"/>
+    <hyperlink ref="G4" r:id="rId6" xr:uid="{665BA96F-F433-485B-9104-A5BA73049A78}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F639E3-C47A-43D0-A8C0-9681F10A43EB}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>80</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>81</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>82</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="10"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="C5" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>83</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>62</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>85</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://www.cuitonline.com/detalle/27452414711/osses-shakira-alejandra.html" xr:uid="{F2232659-C17D-4204-940D-345947882C0E}"/>
+    <hyperlink ref="C5" r:id="rId1" display="https://www.cuitonline.com/detalle/27452414711/osses-shakira-alejandra.html" xr:uid="{F2232659-C17D-4204-940D-345947882C0E}"/>
+    <hyperlink ref="A1" location="menu!A1" display="atras" xr:uid="{6F69DE94-24BD-458D-80F6-2667C9EE1C40}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1650,377 +1754,375 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C54B82-26A3-4EF4-A4EB-E1387A93D0B4}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="B1:W6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J8" sqref="B8:J8"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="0.28515625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" customWidth="1"/>
-    <col min="11" max="11" width="0.28515625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="0.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="0.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.42578125" customWidth="1"/>
+    <col min="12" max="12" width="0.28515625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="4.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>91</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="L1" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="M1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="N1" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>66</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>68</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>69</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>70</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>71</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>72</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>racedo; cristian Damian</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2" t="str">
         <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
         <v>racedo</v>
       </c>
-      <c r="C2" t="str">
+      <c r="D2" t="str">
         <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
         <v>cristian Damian</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>33346</v>
       </c>
-      <c r="E2" s="23" cm="1">
-        <f t="array" aca="1" ref="E2" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
+      <c r="F2" s="23" cm="1">
+        <f t="array" aca="1" ref="F2" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>31</v>
       </c>
-      <c r="F2" s="24">
+      <c r="G2" s="24">
         <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
         <v>31.684931506849313</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="str">
+      <c r="I2" s="6" t="str">
         <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="str">
+      <c r="J2" s="6" t="str">
         <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>35336446</v>
       </c>
-      <c r="J2" s="7" t="str">
+      <c r="K2" s="7" t="str">
         <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>5</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="L2" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="L2" s="26">
+      <c r="M2" s="26">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
         <v>7</v>
       </c>
-      <c r="M2" s="26">
+      <c r="N2" s="26">
         <f>LEN(datos[[#This Row],[empleado]])</f>
         <v>23</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <f ca="1">TODAY()</f>
         <v>44911</v>
       </c>
-      <c r="P2" s="22">
+      <c r="Q2" s="22">
         <f ca="1">NOW()</f>
-        <v>44911.428219675923</v>
-      </c>
-      <c r="Q2">
+        <v>44911.450076851848</v>
+      </c>
+      <c r="R2">
         <f ca="1">YEAR(hoy)</f>
         <v>2022</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <f ca="1">MONTH(hoy)</f>
         <v>12</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <f ca="1">DAY(hoy)</f>
         <v>16</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <f ca="1">HOUR(ahora)</f>
         <v>10</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <f ca="1">MINUTE(ahora)</f>
-        <v>16</v>
-      </c>
-      <c r="V2">
+        <v>48</v>
+      </c>
+      <c r="W2">
         <f ca="1">SECOND(ahora)</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>racedo; Abel Alejandro</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C3" t="str">
         <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
         <v>racedo</v>
       </c>
-      <c r="C3" t="str">
+      <c r="D3" t="str">
         <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
         <v>Abel Alejandro</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>34254</v>
       </c>
-      <c r="E3" s="23" cm="1">
-        <f t="array" aca="1" ref="E3" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
+      <c r="F3" s="23" cm="1">
+        <f t="array" aca="1" ref="F3" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>29</v>
       </c>
-      <c r="F3" s="24">
+      <c r="G3" s="24">
         <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
         <v>29.197260273972603</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="8" t="str">
+      <c r="I3" s="8" t="str">
         <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>20</v>
       </c>
-      <c r="I3" s="8" t="str">
+      <c r="J3" s="8" t="str">
         <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>38558443</v>
       </c>
-      <c r="J3" s="9" t="str">
+      <c r="K3" s="9" t="str">
         <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>6</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="L3" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="L3" s="27">
+      <c r="M3" s="27">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
         <v>7</v>
       </c>
-      <c r="M3" s="27">
+      <c r="N3" s="27">
         <f>LEN(datos[[#This Row],[empleado]])</f>
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="str">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>Aguilera; Cristina</v>
       </c>
-      <c r="B4" t="str">
+      <c r="C4" t="str">
         <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
         <v>Aguilera</v>
       </c>
-      <c r="C4" t="str">
+      <c r="D4" t="str">
         <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
         <v>Cristina</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>29573</v>
       </c>
-      <c r="E4" s="23" cm="1">
-        <f t="array" aca="1" ref="E4" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
+      <c r="F4" s="23" cm="1">
+        <f t="array" aca="1" ref="F4" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>42</v>
       </c>
-      <c r="F4" s="24">
+      <c r="G4" s="24">
         <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
         <v>42.021917808219179</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6" t="str">
+      <c r="I4" s="6" t="str">
         <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>27</v>
       </c>
-      <c r="I4" s="6" t="str">
+      <c r="J4" s="6" t="str">
         <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>14093915</v>
       </c>
-      <c r="J4" s="7" t="str">
+      <c r="K4" s="7" t="str">
         <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>9</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="L4" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="L4" s="26">
+      <c r="M4" s="26">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
         <v>9</v>
       </c>
-      <c r="M4" s="26">
+      <c r="N4" s="26">
         <f>LEN(datos[[#This Row],[empleado]])</f>
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>Osses; Shakira Alejandra</v>
       </c>
-      <c r="B5" t="str">
+      <c r="C5" t="str">
         <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
         <v>Osses</v>
       </c>
-      <c r="C5" t="str">
+      <c r="D5" t="str">
         <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
         <v>Shakira Alejandra</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>28158</v>
       </c>
-      <c r="E5" s="23" cm="1">
-        <f t="array" aca="1" ref="E5" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
+      <c r="F5" s="23" cm="1">
+        <f t="array" aca="1" ref="F5" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>45</v>
       </c>
-      <c r="F5" s="24">
+      <c r="G5" s="24">
         <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
         <v>45.898630136986299</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="H5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="8" t="str">
+      <c r="I5" s="8" t="str">
         <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>27</v>
       </c>
-      <c r="I5" s="8" t="str">
+      <c r="J5" s="8" t="str">
         <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>45241471</v>
       </c>
-      <c r="J5" s="9" t="str">
+      <c r="K5" s="9" t="str">
         <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>1</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="L5" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="L5" s="27">
+      <c r="M5" s="27">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
         <v>6</v>
       </c>
-      <c r="M5" s="27">
+      <c r="N5" s="27">
         <f>LEN(datos[[#This Row],[empleado]])</f>
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" t="str">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>Messi; Lionel Andres</v>
       </c>
-      <c r="B6" t="str">
+      <c r="C6" t="str">
         <f>LEFT(datos[[#This Row],[empleado]],datos[[#This Row],[p]] - 1)</f>
         <v>Messi</v>
       </c>
-      <c r="C6" t="str">
+      <c r="D6" t="str">
         <f>RIGHT(datos[[#This Row],[empleado]],datos[[#This Row],[largo]] - datos[[#This Row],[p]] - 1)</f>
         <v>Lionel Andres</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>31952</v>
       </c>
-      <c r="E6" s="23" cm="1">
-        <f t="array" aca="1" ref="E6" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
+      <c r="F6" s="23" cm="1">
+        <f t="array" aca="1" ref="F6" ca="1">tiempo[AÑO]-YEAR(datos[[#This Row],[NACIMIENTO]])</f>
         <v>35</v>
       </c>
-      <c r="F6" s="24">
+      <c r="G6" s="24">
         <f ca="1">(hoy-datos[[#This Row],[NACIMIENTO]])/365</f>
         <v>35.504109589041093</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="6" t="str">
+      <c r="I6" s="6" t="str">
         <f>LEFT(datos[[#This Row],[CUIL]],2)</f>
         <v>23</v>
       </c>
-      <c r="I6" s="6" t="str">
+      <c r="J6" s="6" t="str">
         <f>MID(datos[[#This Row],[CUIL]],4,8)</f>
         <v>33016244</v>
       </c>
-      <c r="J6" s="7" t="str">
+      <c r="K6" s="7" t="str">
         <f>RIGHT(datos[[#This Row],[CUIL]],1)</f>
         <v>9</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="L6" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="L6" s="26">
+      <c r="M6" s="26">
         <f>FIND(datos[[#This Row],[char]],datos[[#This Row],[empleado]])</f>
         <v>6</v>
       </c>
-      <c r="M6" s="26">
+      <c r="N6" s="26">
         <f>LEN(datos[[#This Row],[empleado]])</f>
         <v>20</v>
       </c>
@@ -2036,193 +2138,190 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FFAE78-438E-4183-90FE-F9F4BDD2CD47}">
-  <dimension ref="A1:AK31"/>
+  <dimension ref="B1:AL31"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="20" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.42578125" style="11" customWidth="1"/>
-    <col min="32" max="32" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="23" max="28" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.7109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="3.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.42578125" style="11" customWidth="1"/>
+    <col min="33" max="33" width="8.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="2:38" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="R1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="T1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="U1" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="W1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="X1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Y1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Z1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AA1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AB1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AD1" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AE1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AF1" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AG1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AH1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>52</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="str">
+    <row r="2" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>racedo; cristian Damian</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="E2" s="14"/>
       <c r="F2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="G2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="15"/>
+      <c r="I2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="14"/>
       <c r="M2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="N2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="15"/>
+      <c r="P2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="14"/>
       <c r="T2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="U2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" s="15"/>
+      <c r="W2" s="14"/>
       <c r="X2" s="14" t="s">
         <v>17</v>
       </c>
@@ -2235,49 +2334,49 @@
       <c r="AA2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="AB2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" s="15"/>
       <c r="AD2" s="14" t="s">
         <v>17</v>
       </c>
       <c r="AE2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AF2" s="18">
-        <f>COUNTA(B2:AE2)</f>
+      <c r="AF2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG2" s="18">
+        <f>COUNTA(C2:AF2)</f>
         <v>19</v>
       </c>
-      <c r="AG2" s="18">
-        <f>COUNTBLANK(B2:AE2)</f>
+      <c r="AH2" s="18">
+        <f>COUNTBLANK(C2:AF2)</f>
         <v>11</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>58</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <f>SUM(presentismo[ASIST])</f>
         <v>88</v>
       </c>
-      <c r="AK2">
+      <c r="AL2">
         <f>SUM(presentismo[AUS])</f>
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="str">
+    <row r="3" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B3" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>racedo; Abel Alejandro</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="11" t="s">
@@ -2286,25 +2385,25 @@
       <c r="K3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="14"/>
+      <c r="L3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="N3" s="14"/>
-      <c r="O3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="14"/>
       <c r="R3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="V3" s="11" t="s">
+      <c r="S3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="W3" s="11" t="s">
@@ -2319,38 +2418,38 @@
       <c r="Z3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF3" s="18">
-        <f t="shared" ref="AF3:AF4" si="0">COUNTA(B3:AE3)</f>
+      <c r="AA3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG3" s="18">
+        <f t="shared" ref="AG3:AG4" si="0">COUNTA(C3:AF3)</f>
         <v>16</v>
       </c>
-      <c r="AG3" s="18">
-        <f t="shared" ref="AG3:AG4" si="1">COUNTBLANK(B3:AE3)</f>
+      <c r="AH3" s="18">
+        <f t="shared" ref="AH3:AH4" si="1">COUNTBLANK(C3:AF3)</f>
         <v>14</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>53</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <f>MAX(presentismo[ASIST])</f>
         <v>19</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <f>MAX(presentismo[AUS])</f>
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="str">
+    <row r="4" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>Aguilera; Cristina</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="C4" s="14"/>
       <c r="D4" s="11" t="s">
         <v>17</v>
       </c>
@@ -2360,23 +2459,23 @@
       <c r="F4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="G4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="11"/>
       <c r="P4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="S4" s="11" t="s">
@@ -2385,10 +2484,10 @@
       <c r="T4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="V4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="X4" s="11" t="s">
+      <c r="U4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="W4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="Y4" s="11" t="s">
@@ -2400,117 +2499,117 @@
       <c r="AA4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AD4" s="11" t="s">
+      <c r="AB4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="AE4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AF4" s="18">
+      <c r="AF4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG4" s="18">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="AG4" s="18">
+      <c r="AH4" s="18">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>54</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <f>MIN(presentismo[ASIST])</f>
         <v>16</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <f>MIN(presentismo[AUS])</f>
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="str">
+    <row r="5" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B5" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>Osses; Shakira Alejandra</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="21" t="s">
+      <c r="C5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
         <v>17</v>
       </c>
       <c r="J5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="S5" s="11" t="s">
+      <c r="K5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="T5" s="14"/>
       <c r="U5" s="14"/>
-      <c r="V5" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="V5" s="14"/>
       <c r="W5" s="14" t="s">
         <v>17</v>
       </c>
       <c r="X5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AA5" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD5" s="11" t="s">
+      <c r="Y5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB5" s="11" t="s">
         <v>64</v>
       </c>
       <c r="AE5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AF5" s="18">
-        <f t="shared" ref="AF5:AF6" si="2">COUNTA(B5:AE5)</f>
+      <c r="AF5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG5" s="18">
+        <f t="shared" ref="AG5:AG6" si="2">COUNTA(C5:AF5)</f>
         <v>16</v>
       </c>
-      <c r="AG5" s="18">
-        <f t="shared" ref="AG5" si="3">COUNTBLANK(B5:AE5)</f>
+      <c r="AH5" s="18">
+        <f t="shared" ref="AH5" si="3">COUNTBLANK(C5:AF5)</f>
         <v>14</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>55</v>
       </c>
-      <c r="AJ5" s="19">
+      <c r="AK5" s="19">
         <f>AVERAGE(presentismo[ASIST])</f>
         <v>17.600000000000001</v>
       </c>
-      <c r="AK5" s="19">
+      <c r="AL5" s="19">
         <f>AVERAGE(presentismo[AUS])</f>
         <v>12.4</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="str">
+    <row r="6" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>Messi; Lionel Andres</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" s="11" t="s">
         <v>17</v>
       </c>
@@ -2520,12 +2619,12 @@
       <c r="E6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="11"/>
-      <c r="I6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="11" t="s">
+      <c r="F6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="11"/>
+      <c r="J6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="L6" s="11" t="s">
@@ -2534,143 +2633,146 @@
       <c r="M6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="R6" s="11" t="s">
+      <c r="N6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="T6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="U6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" s="11"/>
       <c r="W6" s="11" t="s">
         <v>17</v>
       </c>
       <c r="X6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="Z6" s="11" t="s">
-        <v>64</v>
+      <c r="Y6" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="AA6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AC6" s="11" t="s">
+      <c r="AB6" s="11" t="s">
         <v>64</v>
       </c>
       <c r="AD6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AF6" s="18">
+      <c r="AE6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG6" s="18">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="AG6" s="18">
-        <f>COUNTBLANK(B6:AE6)</f>
+      <c r="AH6" s="18">
+        <f>COUNTBLANK(C6:AF6)</f>
         <v>12</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>56</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <f>MEDIAN(presentismo[ASIST])</f>
         <v>18</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <f>MEDIAN(presentismo[AUS])</f>
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="AI7" t="s">
+    <row r="7" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C7" s="14"/>
+      <c r="AJ7" t="s">
         <v>57</v>
       </c>
-      <c r="AJ7">
+      <c r="AK7">
         <f>MODE(presentismo[ASIST])</f>
         <v>19</v>
       </c>
-      <c r="AK7">
+      <c r="AL7">
         <f>MODE(presentismo[AUS])</f>
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B15" s="14"/>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="14"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="14"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="14"/>
+    <row r="8" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2694,263 +2796,259 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3FF01-9040-4806-AC6E-6DE86411CAF8}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="28"/>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>15000</v>
       </c>
-      <c r="F2" s="3">
-        <f t="shared" ref="F2:F11" si="0">cant*precio</f>
+      <c r="G2" s="3">
+        <f t="shared" ref="G2:G11" si="0">cant*precio</f>
         <v>30000</v>
       </c>
-      <c r="G2" s="3">
-        <f t="shared" ref="G2:G11" si="1">total*iva</f>
+      <c r="H2" s="3">
+        <f t="shared" ref="H2:H11" si="1">total*iva</f>
         <v>6300</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <f>total +precio_iva</f>
         <v>36300</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>0.21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3">
         <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>5400</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <f t="shared" si="0"/>
         <v>21600</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <f t="shared" si="1"/>
         <v>4536</v>
       </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H2:H11" si="2">total +precio_iva</f>
+      <c r="I3" s="3">
+        <f t="shared" ref="I2:I11" si="2">total +precio_iva</f>
         <v>26136</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>3800</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <f t="shared" si="0"/>
         <v>11400</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <f t="shared" si="1"/>
         <v>2394</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <f t="shared" si="2"/>
         <v>13794</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>600</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <f t="shared" si="2"/>
         <v>726</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>6</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>8800</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>52800</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <f t="shared" si="1"/>
         <v>11088</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <f t="shared" si="2"/>
         <v>63888</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>10</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>8800</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>88000</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <f t="shared" si="1"/>
         <v>18480</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <f t="shared" si="2"/>
         <v>106480</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>3</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>30</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>600</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>18000</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <f t="shared" si="1"/>
         <v>3780</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <f t="shared" si="2"/>
         <v>21780</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9">
         <v>8</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2958,76 +3056,79 @@
       <c r="D9">
         <v>2</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
         <v>3800</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>7600</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <f t="shared" si="1"/>
         <v>1596</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <f t="shared" si="2"/>
         <v>9196</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>15000</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>3150</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <f t="shared" si="2"/>
         <v>18150</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>1</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3">
         <v>3800</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>7600</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <f t="shared" si="1"/>
         <v>1596</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <f t="shared" si="2"/>
         <v>9196</v>
       </c>
@@ -3035,4 +3136,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A36E50-C0D3-438C-882B-3AEDD4D30357}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Insercion de Imagenes y Formas
</commit_message>
<xml_diff>
--- a/empresa.xlsx
+++ b/empresa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xls-v10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944B5502-3280-4E85-8484-0B17BA5C9AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC59642-C249-45AD-AE65-AFF07FFAE8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBF13C54-EAF5-48F7-B675-6702B08EF7EF}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="112">
   <si>
     <t>codigo</t>
   </si>
@@ -494,7 +494,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -516,6 +516,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -559,7 +565,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -608,25 +614,23 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1073,6 +1077,1240 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>132520</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>50220</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>519311</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>482220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E670DDF4-F253-490A-9DC4-2E8A8BB3DDBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a14:imgLayer r:embed="rId2">
+                  <a14:imgEffect>
+                    <a14:backgroundRemoval t="9930" b="89367" l="10000" r="90000">
+                      <a14:foregroundMark x1="25333" y1="70667" x2="33333" y2="29333"/>
+                      <a14:backgroundMark x1="15111" y1="9778" x2="87556" y2="9778"/>
+                      <a14:backgroundMark x1="14667" y1="14667" x2="6222" y2="76444"/>
+                      <a14:backgroundMark x1="6222" y1="76444" x2="72444" y2="88000"/>
+                      <a14:backgroundMark x1="72444" y1="88000" x2="91556" y2="60444"/>
+                    </a14:backgroundRemoval>
+                  </a14:imgEffect>
+                </a14:imgLayer>
+              </a14:imgProps>
+            </a:ext>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="13580" t="15171" r="10055" b="16457"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="109916" y="72824"/>
+          <a:ext cx="432000" cy="386791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>125072</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>356156</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="430696" cy="1600211"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FD1B155-0DE3-4B86-AD56-256B5D492DDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="-459686" y="940914"/>
+          <a:ext cx="1600211" cy="430696"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1800" b="1" cap="none" spc="50">
+              <a:ln w="9525" cmpd="sng">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="70AD47">
+                  <a:tint val="1000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:glow rad="38100">
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>EDUCACION</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>15812</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>42166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>740353</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>166</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F5DEEC3-1F11-4D86-BCFC-BB12464C38ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:duotone>
+            <a:schemeClr val="accent1">
+              <a:shade val="45000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+            <a:prstClr val="white"/>
+          </a:duotone>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{837473B0-CC2E-450A-ABE3-18F120FF3D39}">
+              <a1611:picAttrSrcUrl xmlns:a1611="http://schemas.microsoft.com/office/drawing/2016/11/main" r:id="rId5"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="22950" r="24218"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4462255" y="994666"/>
+          <a:ext cx="724541" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>70758</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>48986</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>669468</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>734785</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="Grupo 9">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A04C8560-04C7-47AC-B955-FBBEB620BEDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3755742" y="1001486"/>
+          <a:ext cx="598710" cy="685799"/>
+          <a:chOff x="3728358" y="990600"/>
+          <a:chExt cx="598710" cy="685799"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Paralelogramo 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F28F8E8F-8D9B-4263-AF2B-D0BD9D861A6A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="3799114" y="1164771"/>
+            <a:ext cx="527954" cy="419100"/>
+          </a:xfrm>
+          <a:prstGeom prst="parallelogram">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 43182"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+          <a:ln w="76200">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-AR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Paralelogramo 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40BB354E-363F-404C-BF4B-3664E5383121}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3728358" y="990600"/>
+            <a:ext cx="511628" cy="685799"/>
+          </a:xfrm>
+          <a:prstGeom prst="parallelogram">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 66506"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln w="76200">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="es-AR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>13078</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>90469</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733078</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>48469</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Gráfico 13" descr="Maestro con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9996B999-145A-45F4-A720-9E2B239C26A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId9"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2936062" y="1042969"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>14250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>734250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>758063</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Gráfico 15" descr="Lápiz con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47C774A7-A4B7-402D-95C0-D87AF477721A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId12"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2175234" y="990563"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>33281</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>69000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>753281</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>27000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Gráfico 17" descr="Dinero con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3727E697-0789-435B-B83C-209816C8F6CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId15"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3718265" y="69000"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>22547</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>129702</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742547</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>87702</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Gráfico 19" descr="Camión con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEE834ED-922A-4F17-9942-94EAE4346D45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId18"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2945531" y="129702"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>11812</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>23719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>731812</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>743719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Gráfico 21" descr="Correo electrónico con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{143A27E5-9F4C-4CBD-8C66-A337749434C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId21"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1410796" y="976219"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>18937</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>18938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>738937</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>738938</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Gráfico 23" descr="Base de datos con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F38E259-B720-4E3E-8DB3-0198B1659669}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId24"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1417921" y="18938"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>26062</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>43922</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>746062</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1922</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Gráfico 25" descr="Gráfico circular con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1C85EB9-4A4C-4D86-B09C-F77BF5693E9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId27"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4473046" y="43922"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>45093</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>33188</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3093</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>753188</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Gráfico 27" descr="Documento con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA6766F2-19E7-4EF0-888E-110A75FB75A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId30"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="682077" y="985688"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>22452</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>11907</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>742452</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>731907</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Gráfico 29" descr="Identificación de empleado con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46E82619-0467-42A5-AD12-71781D7A70A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId33"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="659436" y="11907"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>29765</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>749765</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>743813</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Gráfico 31" descr="Lista con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AC5E436-E3A7-45D2-B429-62E82AA5F480}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId36"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2190749" y="23813"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>39414</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>13138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219414</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EB9DAF0-CEC1-4DB5-A477-2846CC39CC13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="39414" y="13138"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>39414</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>13138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219414</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B4096E4-E0E7-49B3-9454-D037DEDCBF53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="39414" y="13138"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>39414</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>13138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219414</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>193138</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B4B5927-E67D-4999-AECA-1C0A0C936841}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="39414" y="13138"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>39414</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>13138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219414</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86B46604-226C-47FA-8EE9-C0DCE67E64B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="39414" y="13138"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>39414</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>13138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219414</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3564A81C-29C9-482A-BDEF-D637F58C8B99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="39414" y="13138"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>39414</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>13138</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219414</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Gráfico 1" descr="Atrás con relleno sólido">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD560802-8E10-4783-906C-31CC26948173}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="39414" y="13138"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1511,81 +2749,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBB5BBC-F064-4678-AF8C-C3D428764205}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
     <col min="8" max="8" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H1" s="29" t="s">
+      <c r="A1" s="30"/>
+      <c r="H1" s="33" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="29"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="29" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="33" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="35" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="H4" s="29"/>
+      <c r="H4" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="H3:H4"/>
+    <mergeCell ref="A1:A4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" location="empleados!A1" display="Empleados" xr:uid="{6804FC27-9203-4DBA-8D6C-376C27FE298D}"/>
@@ -1602,6 +2842,7 @@
     <hyperlink ref="G4" r:id="rId6" xr:uid="{665BA96F-F433-485B-9104-A5BA73049A78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1609,7 +2850,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F639E3-C47A-43D0-A8C0-9681F10A43EB}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1633,7 +2877,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>110</v>
       </c>
       <c r="B1" t="s">
@@ -1746,17 +2990,21 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C54B82-26A3-4EF4-A4EB-E1387A93D0B4}">
-  <dimension ref="B1:W6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1775,7 +3023,10 @@
     <col min="14" max="14" width="7.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>110</v>
+      </c>
       <c r="B1" t="s">
         <v>74</v>
       </c>
@@ -1840,7 +3091,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>racedo; cristian Damian</v>
@@ -1896,7 +3147,7 @@
       </c>
       <c r="Q2" s="22">
         <f ca="1">NOW()</f>
-        <v>44911.450076851848</v>
+        <v>44911.487448842592</v>
       </c>
       <c r="R2">
         <f ca="1">YEAR(hoy)</f>
@@ -1912,18 +3163,18 @@
       </c>
       <c r="U2">
         <f ca="1">HOUR(ahora)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="V2">
         <f ca="1">MINUTE(ahora)</f>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="W2">
         <f ca="1">SECOND(ahora)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>racedo; Abel Alejandro</v>
@@ -1974,7 +3225,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>Aguilera; Cristina</v>
@@ -2025,7 +3276,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>Osses; Shakira Alejandra</v>
@@ -2076,7 +3327,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f>TRIM(presentismo[[#This Row],[Empleado]])</f>
         <v>Messi; Lionel Andres</v>
@@ -2128,23 +3379,27 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="menu!A1" display="atras" xr:uid="{C13B0C2E-F2EA-4890-B93A-A2EAF887F4AD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FFAE78-438E-4183-90FE-F9F4BDD2CD47}">
-  <dimension ref="B1:AL31"/>
+  <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +3419,10 @@
     <col min="34" max="34" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>110</v>
+      </c>
       <c r="B1" s="11" t="s">
         <v>16</v>
       </c>
@@ -2274,7 +3532,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>racedo; cristian Damian</v>
@@ -2367,7 +3625,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>racedo; Abel Alejandro</v>
@@ -2444,7 +3702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>Aguilera; Cristina</v>
@@ -2528,7 +3786,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>Osses; Shakira Alejandra</v>
@@ -2605,7 +3863,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="6" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="str">
         <f>_xlfn.CONCAT(empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;empleados[[#This Row],[NOMBRE]])</f>
         <v>Messi; Lionel Andres</v>
@@ -2688,7 +3946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C7" s="14"/>
       <c r="AJ7" t="s">
         <v>57</v>
@@ -2702,31 +3960,31 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C8" s="14"/>
     </row>
-    <row r="9" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C9" s="14"/>
     </row>
-    <row r="10" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C10" s="14"/>
     </row>
-    <row r="11" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C11" s="14"/>
     </row>
-    <row r="12" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C12" s="14"/>
     </row>
-    <row r="13" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C13" s="14"/>
     </row>
-    <row r="14" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C14" s="14"/>
     </row>
-    <row r="15" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C15" s="14"/>
     </row>
-    <row r="16" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="C16" s="14"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
@@ -2775,9 +4033,13 @@
       <c r="C31" s="14"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="menu!A1" display="atras" xr:uid="{F1EAB0D1-36B3-4DE7-8A69-43D9391AAC65}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2786,11 +4048,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BCF59A-9D0C-4ADD-8102-A58A6DC81599}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="menu!A1" display="atras" xr:uid="{0E087567-2D17-47B0-B948-A60227DE6316}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2798,7 +4073,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3FF01-9040-4806-AC6E-6DE86411CAF8}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2811,7 +4089,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
+      <c r="A1" s="31" t="s">
+        <v>110</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3134,7 +4414,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="menu!A1" display="atras" xr:uid="{B77ACD90-79DC-4E97-98F2-9228CD1EFDBA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3142,10 +4426,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A36E50-C0D3-438C-882B-3AEDD4D30357}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="menu!A1" display="atras" xr:uid="{BAEE1280-7C20-467F-A1E1-9F69C0E2B299}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Graficos de Barras y columnas
</commit_message>
<xml_diff>
--- a/empresa.xlsx
+++ b/empresa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xls-v10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D789E5EF-2DA8-465D-854E-EEE984E3B9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F134CF2-E519-4848-97EC-71C28F656C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FBF13C54-EAF5-48F7-B675-6702B08EF7EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6" xr2:uid="{FBF13C54-EAF5-48F7-B675-6702B08EF7EF}"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="6" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="estadisticas" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ventas!$B$1:$I$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">ventas!$B$1:$I$12</definedName>
     <definedName name="ahora">datos!$Q$2</definedName>
     <definedName name="año">datos!$R$2</definedName>
     <definedName name="cant">ventas!$E:$E</definedName>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="149">
   <si>
     <t>codigo</t>
   </si>
@@ -429,21 +429,6 @@
     <t>Mejor vendedor</t>
   </si>
   <si>
-    <t>Producto mas solicitado</t>
-  </si>
-  <si>
-    <t>cantidad ventas</t>
-  </si>
-  <si>
-    <t>Recaudacion total</t>
-  </si>
-  <si>
-    <t>Mediana de ventas</t>
-  </si>
-  <si>
-    <t>Media de ventas</t>
-  </si>
-  <si>
     <t>Descripcion</t>
   </si>
   <si>
@@ -520,6 +505,36 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>ventas</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>promedio</t>
+  </si>
+  <si>
+    <t>mediana</t>
+  </si>
+  <si>
+    <t>moda</t>
+  </si>
+  <si>
+    <t>Producto popular</t>
+  </si>
+  <si>
+    <t>recaudacion</t>
+  </si>
+  <si>
+    <t>recaudado</t>
+  </si>
+  <si>
+    <t>entregado</t>
+  </si>
+  <si>
+    <t>fac</t>
   </si>
 </sst>
 </file>
@@ -532,7 +547,7 @@
     <numFmt numFmtId="164" formatCode="_-[$$-2C0A]\ * #,##0.00_-;\-[$$-2C0A]\ * #,##0.00_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="d/m/yy;@"/>
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -638,7 +653,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -670,6 +685,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -678,7 +713,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -739,19 +774,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Énfasis1" xfId="4" builtinId="29"/>
@@ -760,7 +802,95 @@
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="72">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFCC0066"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -816,25 +946,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="164" formatCode="_-[$$-2C0A]\ * #,##0.00_-;\-[$$-2C0A]\ * #,##0.00_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1392,6 +1504,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC0066"/>
       <color rgb="FFFF7C80"/>
     </mruColors>
   </colors>
@@ -1404,6 +1517,1854 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ventas!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ventas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="70000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>ventas!$L$6:$L$8</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>promedio</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mediana</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>moda</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ventas!$K$6:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>23127.272727272728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E196-404E-8B38-7473E1087FCB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="80"/>
+        <c:overlap val="25"/>
+        <c:axId val="174797663"/>
+        <c:axId val="174796831"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="174797663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="174796831"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="174796831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="174797663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Asistencia</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>P</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>presentismo!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>racedo; cristian Damian</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>racedo; Abel Alejandro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Aguilera; Cristina</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Osses; Shakira Alejandra</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Messi; Lionel Andres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>presentismo!$AG$2:$AG$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5537-4FAB-958F-A1302B527A9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>A</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>presentismo!$B$2:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>racedo; cristian Damian</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>racedo; Abel Alejandro</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Aguilera; Cristina</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Osses; Shakira Alejandra</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Messi; Lionel Andres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>presentismo!$AH$2:$AH$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5537-4FAB-958F-A1302B527A9C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="95"/>
+        <c:overlap val="100"/>
+        <c:axId val="633785151"/>
+        <c:axId val="633786815"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="633785151"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="633786815"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="633786815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="633785151"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="20" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="70000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" i="0" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2521,16 +4482,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>756456</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>54852</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>89666</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>703247</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>173748</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
@@ -2566,7 +4527,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6105525" y="54852"/>
+              <a:off x="10003033" y="0"/>
               <a:ext cx="1470791" cy="2078748"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2599,16 +4560,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>183930</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2094</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>61092</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>599214</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>167507</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
@@ -2644,7 +4605,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7670580" y="61092"/>
+              <a:off x="11534671" y="0"/>
               <a:ext cx="1359120" cy="2072507"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2737,18 +4698,18 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>744192</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:colOff>363191</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="vendedor">
@@ -2771,7 +4732,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -2815,15 +4776,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>405847</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:colOff>901147</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
@@ -2859,7 +4820,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="9429750" y="57151"/>
+              <a:off x="9632673" y="0"/>
               <a:ext cx="1257300" cy="1752600"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2949,6 +4910,80 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E639C38-EEA3-4010-8908-E0C8D54C3230}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07628873-3825-4290-A89F-BB9ABAB55F1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3007,14 +5042,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}" name="Tabla_empleados" displayName="Tabla_empleados" ref="B1:F6" totalsRowShown="0">
-  <autoFilter ref="B1:F6" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9B2FABCB-122E-4021-BCB9-1ABCF38F08D1}" name="CODIGO"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}" name="Tabla_empleados" displayName="Tabla_empleados" ref="B1:H7" totalsRowCount="1">
+  <autoFilter ref="B1:H6" xr:uid="{7DAC5F66-FDAB-4B10-8475-ECE8FAEEF22D}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H6">
+    <sortCondition ref="B1:B6"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{9B2FABCB-122E-4021-BCB9-1ABCF38F08D1}" name="CODIGO" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{48BCCCB0-2E0A-4212-A44B-A72FF9EFADA4}" name="APELLIDO"/>
     <tableColumn id="3" xr3:uid="{8E2D81A4-6B1C-4EE6-B057-EC49A27E5F85}" name="NOMBRE"/>
     <tableColumn id="4" xr3:uid="{FAD0BCDF-63FA-416C-A9FA-7BBA19E4DC2A}" name="LEGAJO"/>
     <tableColumn id="7" xr3:uid="{B0450268-4DC5-4E02-B6A4-0DBA5EAA50A9}" name="SECTOR"/>
+    <tableColumn id="5" xr3:uid="{5A5E88EE-3976-487D-B4E9-E49D2E093EAA}" name="ventas" totalsRowFunction="sum" dataDxfId="8">
+      <calculatedColumnFormula>COUNTIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{308D5340-E507-4A2F-B23C-320C4F3BC1EC}" name="recaudacion" totalsRowFunction="sum" dataCellStyle="Moneda">
+      <calculatedColumnFormula>SUMIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]],Tabla_ventas[total])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3024,10 +5068,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{21CB7767-E429-4D32-8B4C-B110EB0BC09A}" name="tiempo" displayName="tiempo" ref="P1:W2" totalsRowShown="0">
   <autoFilter ref="P1:W2" xr:uid="{21CB7767-E429-4D32-8B4C-B110EB0BC09A}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{D0C157DB-5866-4540-85DA-CA9246E3491C}" name="HOY" dataDxfId="62">
+    <tableColumn id="1" xr3:uid="{D0C157DB-5866-4540-85DA-CA9246E3491C}" name="HOY" dataDxfId="71">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{F19B6CA2-44B0-4AA2-94E5-4821559CF825}" name="AHORA" dataDxfId="61">
+    <tableColumn id="2" xr3:uid="{F19B6CA2-44B0-4AA2-94E5-4821559CF825}" name="AHORA" dataDxfId="70">
       <calculatedColumnFormula>NOW()</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{E5C1B772-C41D-4F28-BDF3-44DE9CE5F354}" name="AÑO">
@@ -3054,40 +5098,40 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A8CA9039-9259-406D-B167-9DC94801EDAB}" name="Tabla_datos" displayName="Tabla_datos" ref="B1:N6" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A8CA9039-9259-406D-B167-9DC94801EDAB}" name="Tabla_datos" displayName="Tabla_datos" ref="B1:N6" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="B1:N6" xr:uid="{A8CA9039-9259-406D-B167-9DC94801EDAB}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{1E40E760-3B7A-46CB-ADE6-9C36221D8FBE}" name="empleado" dataDxfId="58">
+    <tableColumn id="1" xr3:uid="{1E40E760-3B7A-46CB-ADE6-9C36221D8FBE}" name="empleado" dataDxfId="67">
       <calculatedColumnFormula>TRIM(Tabla_presentismo[[#This Row],[Empleado]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A673056C-D666-4A82-8F15-DA591ECD51CD}" name="APELLIDO" dataDxfId="57">
+    <tableColumn id="2" xr3:uid="{A673056C-D666-4A82-8F15-DA591ECD51CD}" name="APELLIDO" dataDxfId="66">
       <calculatedColumnFormula>LEFT(Tabla_datos[[#This Row],[empleado]],Tabla_datos[[#This Row],[p]] - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{98D588C0-9131-404A-823E-4F312157B4EE}" name="NOMBRE" dataDxfId="56">
+    <tableColumn id="3" xr3:uid="{98D588C0-9131-404A-823E-4F312157B4EE}" name="NOMBRE" dataDxfId="65">
       <calculatedColumnFormula>RIGHT(Tabla_datos[[#This Row],[empleado]],Tabla_datos[[#This Row],[largo]] - Tabla_datos[[#This Row],[p]] - 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DA16E63D-3C7B-4235-BC8E-3EB411EC2AF9}" name="NACIMIENTO" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{D65F57BC-8164-4AB7-8337-DE00B9FD8A3A}" name="AÑOS" dataDxfId="54">
+    <tableColumn id="4" xr3:uid="{DA16E63D-3C7B-4235-BC8E-3EB411EC2AF9}" name="NACIMIENTO" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{D65F57BC-8164-4AB7-8337-DE00B9FD8A3A}" name="AÑOS" dataDxfId="63">
       <calculatedColumnFormula array="1">tiempo[AÑO]-YEAR(Tabla_datos[[#This Row],[NACIMIENTO]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{906FCDA3-636B-4283-9205-7AF46F977290}" name="EDAD" dataDxfId="53" dataCellStyle="Millares">
+    <tableColumn id="6" xr3:uid="{906FCDA3-636B-4283-9205-7AF46F977290}" name="EDAD" dataDxfId="62" dataCellStyle="Millares">
       <calculatedColumnFormula>(hoy-Tabla_datos[[#This Row],[NACIMIENTO]])/365</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{019FA1D5-4F09-4717-AE40-B6C31AA7DC9C}" name="CUIL" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{FECB634B-7A6D-4C5C-80DC-9D64C533A46D}" name="G" dataDxfId="51">
+    <tableColumn id="7" xr3:uid="{019FA1D5-4F09-4717-AE40-B6C31AA7DC9C}" name="CUIL" dataDxfId="61"/>
+    <tableColumn id="8" xr3:uid="{FECB634B-7A6D-4C5C-80DC-9D64C533A46D}" name="G" dataDxfId="60">
       <calculatedColumnFormula>LEFT(Tabla_datos[[#This Row],[CUIL]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{4DAF6AA5-E15E-4B0E-A6B3-0413A3FC7025}" name="DOCMENTO" dataDxfId="50">
+    <tableColumn id="9" xr3:uid="{4DAF6AA5-E15E-4B0E-A6B3-0413A3FC7025}" name="DOCMENTO" dataDxfId="59">
       <calculatedColumnFormula>MID(Tabla_datos[[#This Row],[CUIL]],4,8)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{98242B92-44B0-46D8-B255-BEFE9B217C6E}" name="V" dataDxfId="49">
+    <tableColumn id="10" xr3:uid="{98242B92-44B0-46D8-B255-BEFE9B217C6E}" name="V" dataDxfId="58">
       <calculatedColumnFormula>RIGHT(Tabla_datos[[#This Row],[CUIL]],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{96F6AC38-E0D7-4538-BF50-B26B716ECD40}" name="char" dataDxfId="48"/>
-    <tableColumn id="12" xr3:uid="{900EA9DF-7806-4E2A-BE95-A5AA6FF29C93}" name="p" dataDxfId="47">
+    <tableColumn id="11" xr3:uid="{96F6AC38-E0D7-4538-BF50-B26B716ECD40}" name="char" dataDxfId="57"/>
+    <tableColumn id="12" xr3:uid="{900EA9DF-7806-4E2A-BE95-A5AA6FF29C93}" name="p" dataDxfId="56">
       <calculatedColumnFormula>FIND(Tabla_datos[[#This Row],[char]],Tabla_datos[[#This Row],[empleado]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{7A21E3B8-95EE-4371-95D5-EA3889520837}" name="largo" dataDxfId="46">
+    <tableColumn id="13" xr3:uid="{7A21E3B8-95EE-4371-95D5-EA3889520837}" name="largo" dataDxfId="55">
       <calculatedColumnFormula>LEN(Tabla_datos[[#This Row],[empleado]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3096,46 +5140,46 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}" name="Tabla_presentismo" displayName="Tabla_presentismo" ref="B1:AH6" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}" name="Tabla_presentismo" displayName="Tabla_presentismo" ref="B1:AH6" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <autoFilter ref="B1:AH6" xr:uid="{5F56470C-30B4-4EBD-BFC4-C92DB644C2CF}"/>
   <tableColumns count="33">
-    <tableColumn id="1" xr3:uid="{83429F3A-0633-41B4-A217-0D30DFCF116B}" name="Empleado" dataDxfId="43">
+    <tableColumn id="1" xr3:uid="{83429F3A-0633-41B4-A217-0D30DFCF116B}" name="Empleado" dataDxfId="52">
       <calculatedColumnFormula>_xlfn.CONCAT(Tabla_empleados[[#This Row],[APELLIDO]]&amp;"; "&amp;Tabla_empleados[[#This Row],[NOMBRE]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{887EC86C-1521-40B0-A6C3-0B2B3230C024}" name="1/11/22" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{C8618297-DB24-4382-BD1E-E53E7DB10A63}" name="2/11/22" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{6182BB9D-62C7-4740-9A83-3BF4CE62D8C0}" name="3/11/22" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{C4722C79-3465-44B4-AAFE-AED718DFEF78}" name="4/11/22" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{443CA749-360E-405C-BCF0-3AA088ECB546}" name="5/11/22" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{DDC8BC93-6522-4621-A6CE-E663DAA5E060}" name="6/11/22" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{044D1592-31CC-4BD8-9305-F821CBDE87C3}" name="7/11/22" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{58B8F006-DDC6-45D4-913C-A9728CE4DEEB}" name="8/11/22" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{2E67B63B-C7A3-4447-B240-2206A83EB1AE}" name="9/11/22" dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{E063B5BB-2482-4A97-B99C-CEE9E8FBC8AD}" name="10/11/22" dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{C388062D-2D19-400D-9799-432AF612D74D}" name="11/11/22" dataDxfId="32"/>
-    <tableColumn id="13" xr3:uid="{AC73BB9A-6A78-4DB1-885C-194594FB6F10}" name="12/11/22" dataDxfId="31"/>
-    <tableColumn id="14" xr3:uid="{06A3A94F-6999-487D-ABBD-26DFBE539387}" name="13/11/22" dataDxfId="30"/>
-    <tableColumn id="15" xr3:uid="{50DAE1CB-9B50-4836-80C2-0F7D5D1DBF7E}" name="14/11/22" dataDxfId="29"/>
-    <tableColumn id="16" xr3:uid="{BA731102-2D66-4B65-A41F-E60E74E4BC71}" name="15/11/22" dataDxfId="28"/>
-    <tableColumn id="17" xr3:uid="{B971CE8E-7E54-4964-AB64-E900A025F05F}" name="16/11/22" dataDxfId="27"/>
-    <tableColumn id="18" xr3:uid="{F3A47F16-27A5-4C5D-BF2D-83E030C5E47F}" name="17/11/22" dataDxfId="26"/>
-    <tableColumn id="19" xr3:uid="{2DD162DD-96E2-41F4-AD3B-2ACC01BBF7A8}" name="18/11/22" dataDxfId="25"/>
-    <tableColumn id="20" xr3:uid="{55AD600E-9E3F-4481-BAF3-174F391E80B6}" name="19/11/22" dataDxfId="24"/>
-    <tableColumn id="21" xr3:uid="{CB5594F7-50A6-4AB3-8C66-47AE394E8A42}" name="20/11/22" dataDxfId="23"/>
-    <tableColumn id="22" xr3:uid="{9BAC2972-6A5B-4717-B16D-0F035A83C001}" name="21/11/22" dataDxfId="22"/>
-    <tableColumn id="23" xr3:uid="{2C7E1E57-A0FD-43F5-A1C0-D9CEF839010F}" name="22/11/22" dataDxfId="21"/>
-    <tableColumn id="24" xr3:uid="{BF09FF2E-08CF-4C77-B995-FA552B07331C}" name="23/11/22" dataDxfId="20"/>
-    <tableColumn id="25" xr3:uid="{F95FD232-FFA9-4C2A-8A79-A314A99627B1}" name="24/11/22" dataDxfId="19"/>
-    <tableColumn id="26" xr3:uid="{4157B269-FC1E-4344-80EE-594F0938411C}" name="25/11/22" dataDxfId="18"/>
-    <tableColumn id="27" xr3:uid="{500155F2-C488-4E91-95A3-7525D567F566}" name="26/11/22" dataDxfId="17"/>
-    <tableColumn id="28" xr3:uid="{5743E408-8FAC-44AE-81BD-FE1F0BA91CEB}" name="27/11/22" dataDxfId="16"/>
-    <tableColumn id="29" xr3:uid="{919A6993-970F-452F-9B2D-9D06989985BF}" name="28/11/22" dataDxfId="15"/>
-    <tableColumn id="30" xr3:uid="{6FCC3D91-E530-49DC-9803-12984CBA6BE9}" name="29/11/22" dataDxfId="14"/>
-    <tableColumn id="31" xr3:uid="{E6DAAE99-A983-4374-B5B5-FA292704266A}" name="30/11/22" dataDxfId="13"/>
-    <tableColumn id="32" xr3:uid="{9612EC83-2684-4EAF-A263-5FD181F5472E}" name="ASIST" dataDxfId="12">
+    <tableColumn id="2" xr3:uid="{887EC86C-1521-40B0-A6C3-0B2B3230C024}" name="1/11/22" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{C8618297-DB24-4382-BD1E-E53E7DB10A63}" name="2/11/22" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{6182BB9D-62C7-4740-9A83-3BF4CE62D8C0}" name="3/11/22" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{C4722C79-3465-44B4-AAFE-AED718DFEF78}" name="4/11/22" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{443CA749-360E-405C-BCF0-3AA088ECB546}" name="5/11/22" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{DDC8BC93-6522-4621-A6CE-E663DAA5E060}" name="6/11/22" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{044D1592-31CC-4BD8-9305-F821CBDE87C3}" name="7/11/22" dataDxfId="45"/>
+    <tableColumn id="9" xr3:uid="{58B8F006-DDC6-45D4-913C-A9728CE4DEEB}" name="8/11/22" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{2E67B63B-C7A3-4447-B240-2206A83EB1AE}" name="9/11/22" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{E063B5BB-2482-4A97-B99C-CEE9E8FBC8AD}" name="10/11/22" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{C388062D-2D19-400D-9799-432AF612D74D}" name="11/11/22" dataDxfId="41"/>
+    <tableColumn id="13" xr3:uid="{AC73BB9A-6A78-4DB1-885C-194594FB6F10}" name="12/11/22" dataDxfId="40"/>
+    <tableColumn id="14" xr3:uid="{06A3A94F-6999-487D-ABBD-26DFBE539387}" name="13/11/22" dataDxfId="39"/>
+    <tableColumn id="15" xr3:uid="{50DAE1CB-9B50-4836-80C2-0F7D5D1DBF7E}" name="14/11/22" dataDxfId="38"/>
+    <tableColumn id="16" xr3:uid="{BA731102-2D66-4B65-A41F-E60E74E4BC71}" name="15/11/22" dataDxfId="37"/>
+    <tableColumn id="17" xr3:uid="{B971CE8E-7E54-4964-AB64-E900A025F05F}" name="16/11/22" dataDxfId="36"/>
+    <tableColumn id="18" xr3:uid="{F3A47F16-27A5-4C5D-BF2D-83E030C5E47F}" name="17/11/22" dataDxfId="35"/>
+    <tableColumn id="19" xr3:uid="{2DD162DD-96E2-41F4-AD3B-2ACC01BBF7A8}" name="18/11/22" dataDxfId="34"/>
+    <tableColumn id="20" xr3:uid="{55AD600E-9E3F-4481-BAF3-174F391E80B6}" name="19/11/22" dataDxfId="33"/>
+    <tableColumn id="21" xr3:uid="{CB5594F7-50A6-4AB3-8C66-47AE394E8A42}" name="20/11/22" dataDxfId="32"/>
+    <tableColumn id="22" xr3:uid="{9BAC2972-6A5B-4717-B16D-0F035A83C001}" name="21/11/22" dataDxfId="31"/>
+    <tableColumn id="23" xr3:uid="{2C7E1E57-A0FD-43F5-A1C0-D9CEF839010F}" name="22/11/22" dataDxfId="30"/>
+    <tableColumn id="24" xr3:uid="{BF09FF2E-08CF-4C77-B995-FA552B07331C}" name="23/11/22" dataDxfId="29"/>
+    <tableColumn id="25" xr3:uid="{F95FD232-FFA9-4C2A-8A79-A314A99627B1}" name="24/11/22" dataDxfId="28"/>
+    <tableColumn id="26" xr3:uid="{4157B269-FC1E-4344-80EE-594F0938411C}" name="25/11/22" dataDxfId="27"/>
+    <tableColumn id="27" xr3:uid="{500155F2-C488-4E91-95A3-7525D567F566}" name="26/11/22" dataDxfId="26"/>
+    <tableColumn id="28" xr3:uid="{5743E408-8FAC-44AE-81BD-FE1F0BA91CEB}" name="27/11/22" dataDxfId="25"/>
+    <tableColumn id="29" xr3:uid="{919A6993-970F-452F-9B2D-9D06989985BF}" name="28/11/22" dataDxfId="24"/>
+    <tableColumn id="30" xr3:uid="{6FCC3D91-E530-49DC-9803-12984CBA6BE9}" name="29/11/22" dataDxfId="23"/>
+    <tableColumn id="31" xr3:uid="{E6DAAE99-A983-4374-B5B5-FA292704266A}" name="30/11/22" dataDxfId="22"/>
+    <tableColumn id="32" xr3:uid="{9612EC83-2684-4EAF-A263-5FD181F5472E}" name="ASIST" dataDxfId="21">
       <calculatedColumnFormula>COUNTA(C2:AF2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{CF4CC9FE-4916-47D6-BF2F-CC31868C00D4}" name="AUS" dataDxfId="11">
+    <tableColumn id="33" xr3:uid="{CF4CC9FE-4916-47D6-BF2F-CC31868C00D4}" name="AUS" dataDxfId="20">
       <calculatedColumnFormula>COUNTBLANK(C2:AF2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3144,37 +5188,35 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3D377C96-8576-4B15-BA17-2BD00049CD30}" name="Tabla_productos" displayName="Tabla_productos" ref="B1:G10" totalsRowShown="0">
-  <autoFilter ref="B1:G10" xr:uid="{3D377C96-8576-4B15-BA17-2BD00049CD30}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3D377C96-8576-4B15-BA17-2BD00049CD30}" name="Tabla_productos" displayName="Tabla_productos" ref="B1:J11" totalsRowCount="1">
+  <autoFilter ref="B1:J10" xr:uid="{3D377C96-8576-4B15-BA17-2BD00049CD30}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G6">
     <sortCondition ref="B1:B6"/>
   </sortState>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{19D818B5-BCFA-46E0-9471-293C1526FBFE}" name="codigo"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{19D818B5-BCFA-46E0-9471-293C1526FBFE}" name="codigo" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{8D23CB7C-A514-4DDD-B24A-84FC2BD4348C}" name="Descripcion"/>
     <tableColumn id="5" xr3:uid="{537A129A-9889-46D9-8F7B-AF31B4ECDA4F}" name="Categoria"/>
     <tableColumn id="6" xr3:uid="{B207637B-3D2B-4A4A-BC6D-E88E8AF9C86F}" name="Marca"/>
-    <tableColumn id="3" xr3:uid="{AC6F69EE-E287-486C-93CE-CB4F0DFE213C}" name="precio" dataDxfId="6" dataCellStyle="Moneda"/>
+    <tableColumn id="3" xr3:uid="{AC6F69EE-E287-486C-93CE-CB4F0DFE213C}" name="precio" dataDxfId="19" totalsRowDxfId="1" dataCellStyle="Moneda"/>
     <tableColumn id="4" xr3:uid="{2810369F-142D-4CC6-B71E-B4100767C960}" name="Stock"/>
+    <tableColumn id="7" xr3:uid="{BF025DB5-5F89-4ADF-BA18-00E704CB1F7C}" name="fac" totalsRowFunction="sum" dataDxfId="3">
+      <calculatedColumnFormula>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{F00FB435-5F53-4BEE-AF26-4616548A6346}" name="entregado" totalsRowFunction="average" dataDxfId="2" totalsRowDxfId="0">
+      <calculatedColumnFormula>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{BAC4F684-90C7-4213-9814-4846668B68A5}" name="recaudado" totalsRowFunction="sum" dataCellStyle="Moneda">
+      <calculatedColumnFormula>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46713EBC-B864-45CC-8B85-091131957A0F}" name="Tabla_ventas" displayName="Tabla_ventas" ref="B1:I12" totalsRowCount="1" headerRowDxfId="7" dataDxfId="8" headerRowCellStyle="Moneda" dataCellStyle="Moneda">
-  <autoFilter ref="B1:I11" xr:uid="{8CD3FF01-9040-4806-AC6E-6DE86411CAF8}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="4"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{46713EBC-B864-45CC-8B85-091131957A0F}" name="Tabla_ventas" displayName="Tabla_ventas" ref="B1:I12" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Moneda" dataCellStyle="Moneda">
+  <autoFilter ref="B1:I12" xr:uid="{8CD3FF01-9040-4806-AC6E-6DE86411CAF8}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I11">
     <sortCondition ref="B1:B11"/>
   </sortState>
@@ -3183,14 +5225,14 @@
     <tableColumn id="2" xr3:uid="{B5B3A760-4E23-4C46-A4D9-83EB9C7AA444}" name="vendedor"/>
     <tableColumn id="3" xr3:uid="{2BCCB3FC-114B-4ABF-8B8A-4699E7E05B7A}" name="producto"/>
     <tableColumn id="4" xr3:uid="{382CB23A-8AA8-4F37-A270-4ECBE08338DF}" name="cant"/>
-    <tableColumn id="5" xr3:uid="{0E820465-6116-42AB-B3CF-5577B88E0317}" name="precio" totalsRowFunction="countNums" dataDxfId="10" totalsRowDxfId="2" dataCellStyle="Moneda"/>
-    <tableColumn id="6" xr3:uid="{99144CA1-4D07-4C46-89AF-C64FF2EC5C32}" name="total" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="0" dataCellStyle="Moneda">
+    <tableColumn id="5" xr3:uid="{0E820465-6116-42AB-B3CF-5577B88E0317}" name="precio" totalsRowFunction="countNums" dataDxfId="16" totalsRowDxfId="9" dataCellStyle="Moneda"/>
+    <tableColumn id="6" xr3:uid="{99144CA1-4D07-4C46-89AF-C64FF2EC5C32}" name="total" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="10" dataCellStyle="Moneda">
       <calculatedColumnFormula>cant*precio</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5B78A9FD-6297-4C03-91CC-D40B43A95930}" name="iva" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="1" dataCellStyle="Moneda">
+    <tableColumn id="7" xr3:uid="{5B78A9FD-6297-4C03-91CC-D40B43A95930}" name="iva" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="11" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla_ventas[[#This Row],[total]]*iva</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ED091CDD-F115-4839-B377-BE458A5E65A1}" name="final" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3" dataCellStyle="Moneda" totalsRowCellStyle="Moneda">
+    <tableColumn id="8" xr3:uid="{ED091CDD-F115-4839-B377-BE458A5E65A1}" name="final" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla_ventas[[#This Row],[total]] +Tabla_ventas[[#This Row],[iva]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3497,7 +5539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBB5BBC-F064-4678-AF8C-C3D428764205}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
@@ -3508,13 +5550,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33"/>
-      <c r="H1" s="32" t="s">
+      <c r="A1" s="37"/>
+      <c r="H1" s="36" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
+      <c r="A2" s="37"/>
       <c r="B2" s="29" t="s">
         <v>98</v>
       </c>
@@ -3533,22 +5575,22 @@
       <c r="G2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="32"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="36" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="29" t="s">
         <v>103</v>
       </c>
@@ -3567,7 +5609,7 @@
       <c r="G4" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="H4" s="32"/>
+      <c r="H4" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3596,25 +5638,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F639E3-C47A-43D0-A8C0-9681F10A43EB}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.42578125" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
@@ -3624,7 +5665,7 @@
     <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>110</v>
       </c>
@@ -3643,8 +5684,14 @@
       <c r="F1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -3660,8 +5707,23 @@
       <c r="F2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f>COUNTIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]])</f>
+        <v>4</v>
+      </c>
+      <c r="H2" s="32">
+        <f>SUMIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]],Tabla_ventas[total])</f>
+        <v>57400</v>
+      </c>
+      <c r="J2" s="32">
+        <f>SUM(Tabla_empleados[recaudacion])</f>
+        <v>254400</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -3677,8 +5739,23 @@
       <c r="F3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f>COUNTIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]])</f>
+        <v>3</v>
+      </c>
+      <c r="H3" s="32">
+        <f>SUMIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]],Tabla_ventas[total])</f>
+        <v>34000</v>
+      </c>
+      <c r="J3" s="32">
+        <f>AVERAGE(Tabla_empleados[recaudacion])</f>
+        <v>50880</v>
+      </c>
+      <c r="K3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -3694,9 +5771,23 @@
       <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="10">
+        <f>COUNTIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]])</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="32">
+        <f>SUMIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]],Tabla_ventas[total])</f>
+        <v>21600</v>
+      </c>
+      <c r="J4" s="32">
+        <f>MEDIAN(Tabla_empleados[recaudacion])</f>
+        <v>34000</v>
+      </c>
+      <c r="K4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -3712,8 +5803,23 @@
       <c r="F5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f>COUNTIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]])</f>
+        <v>2</v>
+      </c>
+      <c r="H5" s="32">
+        <f>SUMIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]],Tabla_ventas[total])</f>
+        <v>140800</v>
+      </c>
+      <c r="J5" s="32" t="e">
+        <f>MODE(Tabla_empleados[recaudacion])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -3728,6 +5834,27 @@
       </c>
       <c r="F6" t="s">
         <v>65</v>
+      </c>
+      <c r="G6">
+        <f>COUNTIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]])</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="32">
+        <f>SUMIF(Tabla_ventas[vendedor],Tabla_empleados[[#This Row],[CODIGO]],Tabla_ventas[total])</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7">
+        <f>SUBTOTAL(109,Tabla_empleados[ventas])</f>
+        <v>11</v>
+      </c>
+      <c r="H7" s="32">
+        <f>SUBTOTAL(109,Tabla_empleados[recaudacion])</f>
+        <v>254400</v>
       </c>
     </row>
   </sheetData>
@@ -3747,11 +5874,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C54B82-26A3-4EF4-A4EB-E1387A93D0B4}">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3761,7 +5888,7 @@
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="6" max="6" width="0.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -3861,7 +5988,7 @@
       </c>
       <c r="G2" s="24">
         <f ca="1">(hoy-Tabla_datos[[#This Row],[NACIMIENTO]])/365</f>
-        <v>31.684931506849313</v>
+        <v>31.717808219178082</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>6</v>
@@ -3891,11 +6018,11 @@
       </c>
       <c r="P2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44911</v>
+        <v>44923</v>
       </c>
       <c r="Q2" s="22">
         <f ca="1">NOW()</f>
-        <v>44911.539798148151</v>
+        <v>44923.605030787039</v>
       </c>
       <c r="R2">
         <f ca="1">YEAR(hoy)</f>
@@ -3907,19 +6034,19 @@
       </c>
       <c r="T2">
         <f ca="1">DAY(hoy)</f>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="U2">
         <f ca="1">HOUR(ahora)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="V2">
         <f ca="1">MINUTE(ahora)</f>
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="W2">
         <f ca="1">SECOND(ahora)</f>
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -3944,7 +6071,7 @@
       </c>
       <c r="G3" s="24">
         <f ca="1">(hoy-Tabla_datos[[#This Row],[NACIMIENTO]])/365</f>
-        <v>29.197260273972603</v>
+        <v>29.230136986301371</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>5</v>
@@ -3995,7 +6122,7 @@
       </c>
       <c r="G4" s="24">
         <f ca="1">(hoy-Tabla_datos[[#This Row],[NACIMIENTO]])/365</f>
-        <v>42.021917808219179</v>
+        <v>42.054794520547944</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>15</v>
@@ -4046,7 +6173,7 @@
       </c>
       <c r="G5" s="24">
         <f ca="1">(hoy-Tabla_datos[[#This Row],[NACIMIENTO]])/365</f>
-        <v>45.898630136986299</v>
+        <v>45.93150684931507</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>59</v>
@@ -4097,7 +6224,7 @@
       </c>
       <c r="G6" s="24">
         <f ca="1">(hoy-Tabla_datos[[#This Row],[NACIMIENTO]])/365</f>
-        <v>35.504109589041093</v>
+        <v>35.536986301369865</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>60</v>
@@ -4126,15 +6253,56 @@
         <v>20</v>
       </c>
     </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="e">
+        <f>TRIM(Tabla_presentismo[[#This Row],[Empleado]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="41" t="e">
+        <f>FIND(Tabla_datos[[#This Row],[char]],Tabla_datos[[#This Row],[empleado]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N7" s="41" t="e">
+        <f>LEN(Tabla_datos[[#This Row],[empleado]])</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="I2:I6">
+    <cfRule type="beginsWith" dxfId="7" priority="3" operator="beginsWith" text="27">
+      <formula>LEFT(I2,LEN("27"))="27"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="6" priority="4" operator="beginsWith" text="20">
+      <formula>LEFT(I2,LEN("20"))="20"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G6">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>70</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>18</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="menu!A1" display="atras" xr:uid="{C13B0C2E-F2EA-4890-B93A-A2EAF887F4AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4144,10 +6312,10 @@
   <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="AG2" activeCellId="1" sqref="B2:B6 AG2:AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4794,11 +6962,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BCF59A-9D0C-4ADD-8102-A58A6DC81599}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4807,11 +6975,15 @@
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>110</v>
       </c>
@@ -4819,33 +6991,42 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="H1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F2" s="3">
         <v>5400</v>
@@ -4853,19 +7034,38 @@
       <c r="G2">
         <v>6500</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</f>
+        <v>4</v>
+      </c>
+      <c r="J2" s="32">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</f>
+        <v>21600</v>
+      </c>
+      <c r="L2" s="32">
+        <f>SUM(Tabla_productos[recaudado])</f>
+        <v>252600</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F3" s="3">
         <v>3800</v>
@@ -4873,19 +7073,38 @@
       <c r="G3">
         <v>5000</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</f>
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</f>
+        <v>7</v>
+      </c>
+      <c r="J3" s="32">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</f>
+        <v>26600</v>
+      </c>
+      <c r="L3" s="32">
+        <f>AVERAGE(Tabla_productos[recaudado])</f>
+        <v>28066.666666666668</v>
+      </c>
+      <c r="M3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F4" s="3">
         <v>600</v>
@@ -4893,39 +7112,77 @@
       <c r="G4">
         <v>8500</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</f>
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</f>
+        <v>31</v>
+      </c>
+      <c r="J4" s="32">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</f>
+        <v>18600</v>
+      </c>
+      <c r="L4" s="32">
+        <f>MEDIAN(Tabla_productos[recaudado])</f>
+        <v>18600</v>
+      </c>
+      <c r="M4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F5" s="3">
         <v>8800</v>
       </c>
       <c r="G5">
-        <v>6280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3280</v>
+      </c>
+      <c r="H5">
+        <f>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</f>
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</f>
+        <v>16</v>
+      </c>
+      <c r="J5" s="32">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</f>
+        <v>140800</v>
+      </c>
+      <c r="L5" s="32">
+        <f>MODE(Tabla_productos[recaudado])</f>
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F6" s="3">
         <v>15000</v>
@@ -4933,39 +7190,63 @@
       <c r="G6">
         <v>2950</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</f>
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</f>
+        <v>3</v>
+      </c>
+      <c r="J6" s="32">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F7" s="3">
         <v>600</v>
       </c>
       <c r="G7">
-        <v>9920</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4920</v>
+      </c>
+      <c r="H7">
+        <f>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</f>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="32">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E8" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F8" s="3">
         <v>45999.99</v>
@@ -4973,39 +7254,63 @@
       <c r="G8">
         <v>6420</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="32">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E9" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F9" s="3">
         <v>32500</v>
       </c>
       <c r="G9">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2500</v>
+      </c>
+      <c r="H9">
+        <f>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="32">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E10" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F10" s="3">
         <v>120000</v>
@@ -5013,8 +7318,57 @@
       <c r="G10">
         <v>10500</v>
       </c>
+      <c r="H10">
+        <f>COUNTIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]])</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[cant])</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="32">
+        <f>SUMIF(Tabla_ventas[producto],Tabla_productos[[#This Row],[codigo]],Tabla_ventas[total])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="47"/>
+      <c r="H11">
+        <f>SUBTOTAL(109,Tabla_productos[fac])</f>
+        <v>10</v>
+      </c>
+      <c r="I11" s="19">
+        <f>SUBTOTAL(101,Tabla_productos[entregado])</f>
+        <v>6.7777777777777777</v>
+      </c>
+      <c r="J11" s="46">
+        <f>SUBTOTAL(109,Tabla_productos[recaudado])</f>
+        <v>252600</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:F10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G10">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="3000"/>
+        <cfvo type="num" val="6000"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="menu!A1" display="atras" xr:uid="{0E087567-2D17-47B0-B948-A60227DE6316}"/>
   </hyperlinks>
@@ -5035,11 +7389,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD3FF01-9040-4806-AC6E-6DE86411CAF8}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5049,10 +7403,10 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="2.85546875" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5088,7 +7442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -5105,7 +7459,7 @@
         <v>15000</v>
       </c>
       <c r="G2" s="3">
-        <f>cant*precio</f>
+        <f t="shared" ref="G2:G11" si="0">cant*precio</f>
         <v>30000</v>
       </c>
       <c r="H2" s="3">
@@ -5120,12 +7474,12 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -5137,7 +7491,7 @@
         <v>5400</v>
       </c>
       <c r="G3" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>21600</v>
       </c>
       <c r="H3" s="3">
@@ -5151,8 +7505,11 @@
       <c r="K3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -5169,7 +7526,7 @@
         <v>3800</v>
       </c>
       <c r="G4" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>11400</v>
       </c>
       <c r="H4" s="3">
@@ -5180,20 +7537,20 @@
         <f>Tabla_ventas[[#This Row],[total]] +Tabla_ventas[[#This Row],[iva]]</f>
         <v>13794</v>
       </c>
-      <c r="K4" s="35">
+      <c r="K4" s="33">
         <f>COUNT(total)</f>
         <v>11</v>
       </c>
       <c r="L4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -5205,7 +7562,7 @@
         <v>600</v>
       </c>
       <c r="G5" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>600</v>
       </c>
       <c r="H5" s="3">
@@ -5216,20 +7573,20 @@
         <f>Tabla_ventas[[#This Row],[total]] +Tabla_ventas[[#This Row],[iva]]</f>
         <v>726</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5" s="32">
         <f>SUM(total)</f>
-        <v>340600</v>
+        <v>254400</v>
       </c>
       <c r="L5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -5241,7 +7598,7 @@
         <v>8800</v>
       </c>
       <c r="G6" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>52800</v>
       </c>
       <c r="H6" s="3">
@@ -5252,12 +7609,12 @@
         <f>Tabla_ventas[[#This Row],[total]] +Tabla_ventas[[#This Row],[iva]]</f>
         <v>63888</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="32">
         <f>AVERAGE(total)</f>
-        <v>30963.636363636364</v>
+        <v>23127.272727272728</v>
       </c>
       <c r="L6" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -5265,7 +7622,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -5277,7 +7634,7 @@
         <v>8800</v>
       </c>
       <c r="G7" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>88000</v>
       </c>
       <c r="H7" s="3">
@@ -5288,15 +7645,15 @@
         <f>Tabla_ventas[[#This Row],[total]] +Tabla_ventas[[#This Row],[iva]]</f>
         <v>106480</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7" s="32">
         <f>MEDIAN(total)</f>
-        <v>18000</v>
+        <v>15000</v>
       </c>
       <c r="L7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
@@ -5313,7 +7670,7 @@
         <v>600</v>
       </c>
       <c r="G8" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>18000</v>
       </c>
       <c r="H8" s="3">
@@ -5324,15 +7681,15 @@
         <f>Tabla_ventas[[#This Row],[total]] +Tabla_ventas[[#This Row],[iva]]</f>
         <v>21780</v>
       </c>
-      <c r="K8" s="35">
-        <f>MODE(C:C)</f>
-        <v>1</v>
+      <c r="K8" s="32">
+        <f>MODE(Tabla_ventas[total])</f>
+        <v>7600</v>
       </c>
       <c r="L8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
@@ -5349,7 +7706,7 @@
         <v>3800</v>
       </c>
       <c r="G9" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>7600</v>
       </c>
       <c r="H9" s="3">
@@ -5360,20 +7717,20 @@
         <f>Tabla_ventas[[#This Row],[total]] +Tabla_ventas[[#This Row],[iva]]</f>
         <v>9196</v>
       </c>
-      <c r="K9" s="35">
-        <f>MODE(D:D)</f>
-        <v>2</v>
+      <c r="K9" s="33">
+        <f>MODE(C:C)</f>
+        <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -5385,7 +7742,7 @@
         <v>15000</v>
       </c>
       <c r="G10" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>15000</v>
       </c>
       <c r="H10" s="3">
@@ -5396,8 +7753,15 @@
         <f>Tabla_ventas[[#This Row],[total]] +Tabla_ventas[[#This Row],[iva]]</f>
         <v>18150</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="33">
+        <f>MODE(D:D)</f>
+        <v>2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
@@ -5414,7 +7778,7 @@
         <v>3800</v>
       </c>
       <c r="G11" s="3">
-        <f>cant*precio</f>
+        <f t="shared" si="0"/>
         <v>7600</v>
       </c>
       <c r="H11" s="3">
@@ -5427,76 +7791,100 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>143</v>
-      </c>
-      <c r="F12" s="39">
-        <f>SUBTOTAL(102,Tabla_ventas[precio])</f>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="G12" s="40">
-        <f>SUBTOTAL(109,Tabla_ventas[total])</f>
-        <v>88000</v>
-      </c>
-      <c r="H12" s="40">
-        <f>SUBTOTAL(109,Tabla_ventas[iva])</f>
-        <v>18480</v>
-      </c>
-      <c r="I12" s="38">
-        <f>SUBTOTAL(109,Tabla_ventas[final])</f>
-        <v>106480</v>
-      </c>
-      <c r="K12" s="37"/>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" s="3">
+        <v>600</v>
+      </c>
+      <c r="G12" s="3">
+        <f>cant*precio</f>
+        <v>1800</v>
+      </c>
+      <c r="H12" s="3">
+        <f>Tabla_ventas[[#This Row],[total]]*iva</f>
+        <v>378</v>
+      </c>
+      <c r="I12" s="3">
+        <f>Tabla_ventas[[#This Row],[total]] +Tabla_ventas[[#This Row],[iva]]</f>
+        <v>2178</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K13" s="37"/>
+      <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K14" s="37"/>
+      <c r="K14" s="35"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K15" s="36"/>
+      <c r="K15" s="35"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K16" s="36"/>
+      <c r="K16" s="34"/>
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17" s="36"/>
+      <c r="K17" s="34"/>
     </row>
     <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="36"/>
+      <c r="K18" s="34"/>
     </row>
     <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19" s="36"/>
+      <c r="K19" s="34"/>
     </row>
     <row r="20" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K20" s="36"/>
+      <c r="K20" s="34"/>
     </row>
     <row r="21" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K21" s="36"/>
+      <c r="K21" s="34"/>
     </row>
     <row r="22" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K22" s="36"/>
+      <c r="K22" s="34"/>
     </row>
     <row r="23" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K23" s="36"/>
+      <c r="K23" s="34"/>
     </row>
     <row r="24" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K24" s="36"/>
+      <c r="K24" s="34"/>
     </row>
     <row r="25" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K25" s="36"/>
+      <c r="K25" s="34"/>
     </row>
     <row r="26" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K26" s="36"/>
+      <c r="K26" s="34"/>
     </row>
     <row r="27" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K27" s="37"/>
+      <c r="K27" s="34"/>
     </row>
     <row r="28" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K28" s="37"/>
+      <c r="K28" s="35"/>
+    </row>
+    <row r="29" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="35"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I2:I12">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{201DF649-FF7E-4AE8-960D-007F7A896E73}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="menu!A1" display="atras" xr:uid="{B77ACD90-79DC-4E97-98F2-9228CD1EFDBA}"/>
   </hyperlinks>
@@ -5506,6 +7894,21 @@
     <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{201DF649-FF7E-4AE8-960D-007F7A896E73}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I2:I12</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
         <x14:slicer r:id="rId3"/>
@@ -5519,9 +7922,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A36E50-C0D3-438C-882B-3AEDD4D30357}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Grafico Circular y Combinado
</commit_message>
<xml_diff>
--- a/empresa.xlsx
+++ b/empresa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\office\Excel\xls-v10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F134CF2-E519-4848-97EC-71C28F656C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DAF9F1-987B-472E-8E72-9B8F90FBD5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="6" xr2:uid="{FBF13C54-EAF5-48F7-B675-6702B08EF7EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="6" xr2:uid="{FBF13C54-EAF5-48F7-B675-6702B08EF7EF}"/>
   </bookViews>
   <sheets>
     <sheet name="menu" sheetId="6" r:id="rId1"/>
@@ -2290,6 +2290,1108 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>empleados!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>recaudacion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.23340048118985116"/>
+                  <c:y val="-9.2592774861475644E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.18611111111111112"/>
+                  <c:y val="0.11111111111111102"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.40833344269466315"/>
+                  <c:y val="6.5225831146106736E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:solidFill>
+                  <a:sysClr val="window" lastClr="FFFFFF"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="25000"/>
+                      <a:lumOff val="75000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-AR"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="roundRect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.26505818022747152"/>
+                      <c:h val="0.1304097404491105"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.18888888888888888"/>
+                  <c:y val="-2.7777777777777863E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.33333333333333331"/>
+                  <c:y val="-6.9444444444444448E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="1"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="roundRect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>empleados!$C$2:$D$6</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>cristian Damian</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Abel Alejandro</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Cristina</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Shakira Alejandra</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Lionel Andres</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>racedo</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>racedo</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Aguilera</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Osses</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Messi</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>empleados!$H$2:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>57400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2731-4E6F-9EA2-1BEF2BD7300D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="75"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-AR"/>
+              <a:t>Estadisticas de Ventas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>empleados!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>recaudacion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-AR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>empleados!$H$2:$H$6</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>57400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BF57-44DC-B437-24C2C861921B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="273245391"/>
+        <c:axId val="273245807"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>empleados!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ventas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>empleados!$C$2:$D$6</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="5"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>cristian Damian</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Abel Alejandro</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Cristina</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Shakira Alejandra</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Lionel Andres</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>racedo</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>racedo</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Aguilera</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Osses</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Messi</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>empleados!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF57-44DC-B437-24C2C861921B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="272200047"/>
+        <c:axId val="272200879"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="272200047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="272200879"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="272200879"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="272200047"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="273245807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-AR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="273245391"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="273245391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="273245807"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-AR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-AR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2370,6 +3472,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="215">
   <cs:axisTitle>
@@ -3335,6 +4517,1028 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4919,7 +7123,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>752474</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -4948,16 +7152,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4979,6 +7183,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>186979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>72679</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD671D6E-0CF0-4BB3-BF18-F7907FFD979A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F0976D3-2201-4B52-AC37-7C4B574BA249}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5640,9 +7918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F639E3-C47A-43D0-A8C0-9681F10A43EB}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2:K5"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6022,7 +8300,7 @@
       </c>
       <c r="Q2" s="22">
         <f ca="1">NOW()</f>
-        <v>44923.605030787039</v>
+        <v>44923.628377777779</v>
       </c>
       <c r="R2">
         <f ca="1">YEAR(hoy)</f>
@@ -6038,15 +8316,15 @@
       </c>
       <c r="U2">
         <f ca="1">HOUR(ahora)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="V2">
         <f ca="1">MINUTE(ahora)</f>
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="W2">
         <f ca="1">SECOND(ahora)</f>
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -6312,7 +8590,7 @@
   <dimension ref="A1:AL31"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AG2" activeCellId="1" sqref="B2:B6 AG2:AH6"/>
@@ -6966,7 +9244,7 @@
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7922,9 +10200,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A36E50-C0D3-438C-882B-3AEDD4D30357}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>